<commit_message>
Support valueset inspection, reset parameter to default
</commit_message>
<xml_diff>
--- a/editor-models/generated-models/src/main/resources/HeD_Templates.xlsx
+++ b/editor-models/generated-models/src/main/resources/HeD_Templates.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="643" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="1" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="643" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Demo Triggers" sheetId="1" state="visible" r:id="rId2"/>
@@ -205,7 +205,7 @@
     <t>codeSystem=SNOMED</t>
   </si>
   <si>
-    <t>Findings</t>
+    <t>Findings, Condition</t>
   </si>
   <si>
     <t>PatientAge</t>
@@ -214,7 +214,7 @@
     <t>Age</t>
   </si>
   <si>
-    <t>Person</t>
+    <t>EvaluatedPerson</t>
   </si>
   <si>
     <t>age</t>
@@ -856,13 +856,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R65536"/>
+  <dimension ref="A1:R14"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="A14" activeCellId="0" pane="topLeft" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.1"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="4" min="1" style="0" width="11.5204081632653"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="33.3418367346939"/>
@@ -1273,7 +1273,7 @@
         <v>37</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="14">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="14">
       <c r="A14" s="0" t="n">
         <v>12</v>
       </c>
@@ -1302,8 +1302,6 @@
         <v>37</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048575"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048576"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -1322,8 +1320,8 @@
   </sheetPr>
   <dimension ref="A1:R49"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="K24" activeCellId="0" pane="topLeft" sqref="K24"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="E3" activeCellId="0" pane="topLeft" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.1"/>

</xml_diff>

<commit_message>
Support NOT in conditional actions
</commit_message>
<xml_diff>
--- a/editor-models/generated-models/src/main/resources/HeD_Templates.xlsx
+++ b/editor-models/generated-models/src/main/resources/HeD_Templates.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="1" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="643" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="2" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="643" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Demo Triggers" sheetId="1" state="visible" r:id="rId2"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="183">
   <si>
     <t>Sequence ID</t>
   </si>
@@ -265,90 +265,93 @@
     <t>Date Range</t>
   </si>
   <si>
+    <t>codeSystem=TBD;code=active;displayValie=ACTIVE</t>
+  </si>
+  <si>
+    <t>ResolvedProblemDiagnosis</t>
+  </si>
+  <si>
+    <t>codeSystem=TBD;code=resolved;displayValue=RESOLVED</t>
+  </si>
+  <si>
+    <t>StatusPostSurgery</t>
+  </si>
+  <si>
+    <t>Procedure</t>
+  </si>
+  <si>
+    <t>procedureTime</t>
+  </si>
+  <si>
+    <t>IVL_TS</t>
+  </si>
+  <si>
+    <t>Orders/Actions, Condition</t>
+  </si>
+  <si>
+    <t>PatientOnMedication</t>
+  </si>
+  <si>
+    <t>Medication</t>
+  </si>
+  <si>
+    <t>SubstanceAdministrationEvent</t>
+  </si>
+  <si>
+    <t>substanceAdministrationGeneralPurpose</t>
+  </si>
+  <si>
+    <t>codeSystem=RXNORM</t>
+  </si>
+  <si>
+    <t>Last Administration</t>
+  </si>
+  <si>
+    <t>administrationTimeInterval</t>
+  </si>
+  <si>
+    <t>Observations/Results,Condition</t>
+  </si>
+  <si>
+    <t>LabTestResultWithThreshold</t>
+  </si>
+  <si>
+    <t>Observed Quantity</t>
+  </si>
+  <si>
+    <t>Threshold</t>
+  </si>
+  <si>
+    <t>observationValue</t>
+  </si>
+  <si>
+    <t>Procedures, Condition</t>
+  </si>
+  <si>
+    <t>LabTestWithinTimeInterval</t>
+  </si>
+  <si>
+    <t>Lab Type</t>
+  </si>
+  <si>
+    <t>Time Interval</t>
+  </si>
+  <si>
+    <t>Non-LabWithinTimeInterval</t>
+  </si>
+  <si>
+    <t>ActiveDiagnosisOfAcuteHeartDisease</t>
+  </si>
+  <si>
+    <t>Cardiac Problem Type</t>
+  </si>
+  <si>
+    <t>SNOMED:127337006</t>
+  </si>
+  <si>
     <t>codeSystem=TBD;code=active</t>
   </si>
   <si>
-    <t>ResolvedProblemDiagnosis</t>
-  </si>
-  <si>
-    <t>codeSystem=TBD;code=resolved</t>
-  </si>
-  <si>
-    <t>StatusPostSurgery</t>
-  </si>
-  <si>
-    <t>Procedure</t>
-  </si>
-  <si>
-    <t>procedureTime</t>
-  </si>
-  <si>
-    <t>IVL_TS</t>
-  </si>
-  <si>
-    <t>Orders/Actions, Condition</t>
-  </si>
-  <si>
-    <t>PatientOnMedication</t>
-  </si>
-  <si>
-    <t>Medication</t>
-  </si>
-  <si>
-    <t>SubstanceAdministrationEvent</t>
-  </si>
-  <si>
-    <t>substanceAdministrationGeneralPurpose</t>
-  </si>
-  <si>
-    <t>codeSystem=RXNORM</t>
-  </si>
-  <si>
-    <t>Last Administration</t>
-  </si>
-  <si>
-    <t>administrationTimeInterval</t>
-  </si>
-  <si>
-    <t>Observations/Results,Condition</t>
-  </si>
-  <si>
-    <t>LabTestResultWithThreshold</t>
-  </si>
-  <si>
-    <t>Observed Quantity</t>
-  </si>
-  <si>
-    <t>Threshold</t>
-  </si>
-  <si>
-    <t>observationValue</t>
-  </si>
-  <si>
-    <t>Procedures</t>
-  </si>
-  <si>
-    <t>LabTestWithinTimeInterval</t>
-  </si>
-  <si>
-    <t>Lab Type</t>
-  </si>
-  <si>
-    <t>Time Interval</t>
-  </si>
-  <si>
-    <t>Non-LabWithinTimeInterval</t>
-  </si>
-  <si>
-    <t>ActiveDiagnosisOfAcuteHeartDisease</t>
-  </si>
-  <si>
-    <t>Cardiac Problem Type</t>
-  </si>
-  <si>
-    <t>SNOMED:127337006</t>
-  </si>
-  <si>
     <t>Communications, Action, Create</t>
   </si>
   <si>
@@ -554,6 +557,15 @@
   </si>
   <si>
     <t>Concept</t>
+  </si>
+  <si>
+    <t>MedicationIntake</t>
+  </si>
+  <si>
+    <t>Drug Taken</t>
+  </si>
+  <si>
+    <t>substance</t>
   </si>
 </sst>
 </file>
@@ -1320,8 +1332,8 @@
   </sheetPr>
   <dimension ref="A1:R49"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="E3" activeCellId="0" pane="topLeft" sqref="E3"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="A34" activeCellId="0" pane="topLeft" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.1"/>
@@ -2014,6 +2026,11 @@
         <v>28</v>
       </c>
     </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="30">
+      <c r="E30" s="0" t="s">
+        <v>102</v>
+      </c>
+    </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="31">
       <c r="A31" s="0" t="n">
         <v>60</v>
@@ -2156,7 +2173,7 @@
         <v>24</v>
       </c>
       <c r="M49" s="0" t="s">
-        <v>82</v>
+        <v>110</v>
       </c>
       <c r="O49" s="0" t="s">
         <v>37</v>
@@ -2180,8 +2197,8 @@
   </sheetPr>
   <dimension ref="A1:ALZ65536"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="D1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="K4" activeCellId="0" pane="topLeft" sqref="K4"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="A38" activeCellId="0" pane="topLeft" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.1"/>
@@ -2248,25 +2265,25 @@
       <c r="C2" s="17"/>
       <c r="D2" s="17"/>
       <c r="E2" s="18" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="H2" s="18" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="I2" s="18" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="J2" s="18" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="K2" s="18" t="s">
         <v>24</v>
       </c>
       <c r="O2" s="18" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="Q2" s="17"/>
       <c r="R2" s="17"/>
@@ -2709,19 +2726,19 @@
       <c r="C3" s="17"/>
       <c r="D3" s="17"/>
       <c r="E3" s="18" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F3" s="17" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="H3" s="18" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="I3" s="18" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="J3" s="18" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="K3" s="18" t="s">
         <v>77</v>
@@ -3170,19 +3187,19 @@
       <c r="C4" s="17"/>
       <c r="D4" s="17"/>
       <c r="E4" s="18" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F4" s="17" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="H4" s="18" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="I4" s="18" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="J4" s="18" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="K4" s="18" t="s">
         <v>77</v>
@@ -3631,19 +3648,19 @@
       <c r="C5" s="17"/>
       <c r="D5" s="17"/>
       <c r="E5" s="18" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F5" s="17" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="H5" s="18" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="I5" s="18" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="J5" s="18" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="K5" s="18" t="s">
         <v>77</v>
@@ -4092,25 +4109,25 @@
       <c r="C6" s="17"/>
       <c r="D6" s="17"/>
       <c r="E6" s="18" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F6" s="17" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="H6" s="18" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="I6" s="18" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="J6" s="18" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="K6" s="18" t="s">
         <v>77</v>
       </c>
       <c r="O6" s="18" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="Q6" s="17"/>
       <c r="R6" s="17"/>
@@ -4553,25 +4570,25 @@
       <c r="C7" s="17"/>
       <c r="D7" s="17"/>
       <c r="E7" s="18" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F7" s="17" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="H7" s="18" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="I7" s="18" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="J7" s="18" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="K7" s="18" t="s">
         <v>77</v>
       </c>
       <c r="O7" s="18" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="Q7" s="17"/>
       <c r="R7" s="17"/>
@@ -5014,25 +5031,25 @@
       <c r="C8" s="17"/>
       <c r="D8" s="17"/>
       <c r="E8" s="18" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F8" s="17" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="H8" s="18" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="I8" s="18" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="J8" s="18" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="K8" s="18" t="s">
         <v>77</v>
       </c>
       <c r="O8" s="18" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="Q8" s="17"/>
       <c r="R8" s="17"/>
@@ -5475,25 +5492,25 @@
       <c r="C9" s="17"/>
       <c r="D9" s="17"/>
       <c r="E9" s="18" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F9" s="17" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="H9" s="18" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="I9" s="18" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="J9" s="18" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="K9" s="18" t="s">
         <v>77</v>
       </c>
       <c r="O9" s="18" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="Q9" s="17"/>
       <c r="R9" s="17"/>
@@ -5936,25 +5953,25 @@
       <c r="C10" s="17"/>
       <c r="D10" s="17"/>
       <c r="E10" s="18" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F10" s="17" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="H10" s="18" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="I10" s="18" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="J10" s="18" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="K10" s="18" t="s">
         <v>77</v>
       </c>
       <c r="O10" s="18" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="Q10" s="17"/>
       <c r="R10" s="17"/>
@@ -6397,25 +6414,25 @@
       <c r="C11" s="17"/>
       <c r="D11" s="17"/>
       <c r="E11" s="18" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F11" s="17" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="H11" s="18" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="I11" s="18" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="J11" s="18" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="K11" s="18" t="s">
         <v>77</v>
       </c>
       <c r="O11" s="18" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="Q11" s="17"/>
       <c r="R11" s="17"/>
@@ -6858,25 +6875,25 @@
       <c r="C12" s="17"/>
       <c r="D12" s="17"/>
       <c r="E12" s="18" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F12" s="17" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="H12" s="18" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="I12" s="18" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="J12" s="18" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="K12" s="18" t="s">
         <v>77</v>
       </c>
       <c r="O12" s="18" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="Q12" s="17"/>
       <c r="R12" s="17"/>
@@ -7319,25 +7336,25 @@
       <c r="C13" s="17"/>
       <c r="D13" s="17"/>
       <c r="E13" s="18" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F13" s="17" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="H13" s="18" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="I13" s="18" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="J13" s="18" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="K13" s="18" t="s">
         <v>77</v>
       </c>
       <c r="O13" s="18" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="Q13" s="17"/>
       <c r="R13" s="17"/>
@@ -7780,19 +7797,19 @@
       <c r="C14" s="19"/>
       <c r="D14" s="17"/>
       <c r="E14" s="18" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F14" s="17" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="H14" s="18" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="I14" s="18" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="J14" s="18" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="K14" s="18" t="s">
         <v>77</v>
@@ -8241,20 +8258,20 @@
       <c r="C15" s="20"/>
       <c r="D15" s="17"/>
       <c r="E15" s="21" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F15" s="22" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="G15" s="21"/>
       <c r="H15" s="18" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="I15" s="18" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="J15" s="18" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="K15" s="18" t="s">
         <v>57</v>
@@ -8296,20 +8313,20 @@
       <c r="C16" s="20"/>
       <c r="D16" s="17"/>
       <c r="E16" s="21" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F16" s="22" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="G16" s="21"/>
       <c r="H16" s="18" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="I16" s="18" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="J16" s="18" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="K16" s="18" t="s">
         <v>77</v>
@@ -8351,20 +8368,20 @@
       <c r="C17" s="20"/>
       <c r="D17" s="17"/>
       <c r="E17" s="21" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F17" s="22" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="G17" s="21"/>
       <c r="H17" s="18" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="I17" s="18" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="J17" s="18" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="K17" s="18" t="s">
         <v>77</v>
@@ -8406,20 +8423,20 @@
       <c r="C18" s="20"/>
       <c r="D18" s="17"/>
       <c r="E18" s="21" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F18" s="22" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="G18" s="21"/>
       <c r="H18" s="18" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="I18" s="18" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="J18" s="18" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="K18" s="18" t="s">
         <v>77</v>
@@ -8461,20 +8478,20 @@
       <c r="C19" s="20"/>
       <c r="D19" s="17"/>
       <c r="E19" s="21" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F19" s="22" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="G19" s="21"/>
       <c r="H19" s="18" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="I19" s="18" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="J19" s="18" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="K19" s="18" t="s">
         <v>77</v>
@@ -8483,7 +8500,7 @@
       <c r="M19" s="18"/>
       <c r="N19" s="18"/>
       <c r="O19" s="18" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="P19" s="18"/>
       <c r="Q19" s="17"/>
@@ -8516,17 +8533,17 @@
       <c r="C20" s="20"/>
       <c r="D20" s="17"/>
       <c r="E20" s="21" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F20" s="22" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="G20" s="21"/>
       <c r="H20" s="18" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="I20" s="18" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="J20" s="18" t="s">
         <v>96</v>
@@ -8571,20 +8588,20 @@
       <c r="C21" s="20"/>
       <c r="D21" s="17"/>
       <c r="E21" s="21" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F21" s="22" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="G21" s="21"/>
       <c r="H21" s="18" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="I21" s="18" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="J21" s="18" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="K21" s="18" t="s">
         <v>77</v>
@@ -8625,20 +8642,20 @@
       <c r="C22" s="20"/>
       <c r="D22" s="17"/>
       <c r="E22" s="21" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F22" s="22" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="G22" s="21"/>
       <c r="H22" s="18" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="I22" s="18" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="J22" s="18" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="K22" s="18" t="s">
         <v>77</v>
@@ -8647,7 +8664,7 @@
       <c r="M22" s="18"/>
       <c r="N22" s="18"/>
       <c r="O22" s="18" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="P22" s="18"/>
       <c r="Q22" s="17"/>
@@ -8680,20 +8697,20 @@
       <c r="C23" s="20"/>
       <c r="D23" s="17"/>
       <c r="E23" s="21" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F23" s="22" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="G23" s="21"/>
       <c r="H23" s="18" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="I23" s="18" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="J23" s="18" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="K23" s="18" t="s">
         <v>77</v>
@@ -8702,7 +8719,7 @@
       <c r="M23" s="18"/>
       <c r="N23" s="18"/>
       <c r="O23" s="18" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="P23" s="18"/>
       <c r="Q23" s="17"/>
@@ -8735,17 +8752,17 @@
       <c r="C24" s="20"/>
       <c r="D24" s="17"/>
       <c r="E24" s="21" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F24" s="22" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="G24" s="21"/>
       <c r="H24" s="18" t="s">
         <v>22</v>
       </c>
       <c r="I24" s="18" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="J24" s="18" t="s">
         <v>23</v>
@@ -8790,20 +8807,20 @@
       <c r="C25" s="20"/>
       <c r="D25" s="17"/>
       <c r="E25" s="21" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F25" s="22" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="G25" s="21"/>
       <c r="H25" s="18" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="I25" s="18" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="J25" s="18" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="K25" s="18" t="s">
         <v>77</v>
@@ -8845,20 +8862,20 @@
       <c r="C26" s="20"/>
       <c r="D26" s="17"/>
       <c r="E26" s="21" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F26" s="22" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="G26" s="21"/>
       <c r="H26" s="18" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="I26" s="18" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="J26" s="18" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="K26" s="18" t="s">
         <v>77</v>
@@ -8867,7 +8884,7 @@
       <c r="M26" s="18"/>
       <c r="N26" s="18"/>
       <c r="O26" s="18" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="P26" s="18"/>
       <c r="Q26" s="17"/>
@@ -8900,20 +8917,20 @@
       <c r="C27" s="20"/>
       <c r="D27" s="9"/>
       <c r="E27" s="21" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F27" s="22" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="G27" s="21"/>
       <c r="H27" s="18" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="I27" s="18" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="J27" s="18" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="K27" s="18" t="s">
         <v>57</v>
@@ -8955,20 +8972,20 @@
       <c r="C28" s="20"/>
       <c r="D28" s="9"/>
       <c r="E28" s="21" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F28" s="22" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="G28" s="21"/>
       <c r="H28" s="18" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="I28" s="18" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="J28" s="21" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="K28" s="21" t="s">
         <v>77</v>
@@ -9010,20 +9027,20 @@
       <c r="C29" s="20"/>
       <c r="D29" s="9"/>
       <c r="E29" s="21" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F29" s="22" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="G29" s="21"/>
       <c r="H29" s="18" t="s">
+        <v>174</v>
+      </c>
+      <c r="I29" s="18" t="s">
         <v>173</v>
       </c>
-      <c r="I29" s="18" t="s">
-        <v>172</v>
-      </c>
       <c r="J29" s="18" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="K29" s="18" t="s">
         <v>77</v>
@@ -9065,20 +9082,20 @@
       <c r="C30" s="20"/>
       <c r="D30" s="9"/>
       <c r="E30" s="21" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F30" s="22" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="G30" s="22"/>
       <c r="H30" s="17" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="I30" s="18" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="J30" s="17" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="K30" s="17" t="s">
         <v>77</v>
@@ -9119,20 +9136,20 @@
       <c r="C31" s="20"/>
       <c r="D31" s="9"/>
       <c r="E31" s="21" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F31" s="22" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="G31" s="21"/>
       <c r="H31" s="18" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="I31" s="18" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="J31" s="18" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="K31" s="18" t="s">
         <v>77</v>
@@ -9141,7 +9158,7 @@
       <c r="M31" s="18"/>
       <c r="N31" s="18"/>
       <c r="O31" s="18" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="P31" s="18"/>
       <c r="Q31" s="17"/>
@@ -9174,20 +9191,20 @@
       <c r="C32" s="20"/>
       <c r="D32" s="9"/>
       <c r="E32" s="21" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F32" s="22" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="G32" s="21"/>
       <c r="H32" s="18" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="I32" s="18" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="J32" s="18" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="K32" s="18" t="s">
         <v>77</v>
@@ -9196,7 +9213,7 @@
       <c r="M32" s="18"/>
       <c r="N32" s="18"/>
       <c r="O32" s="18" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="P32" s="18"/>
       <c r="Q32" s="17"/>
@@ -9229,20 +9246,20 @@
       <c r="C33" s="20"/>
       <c r="D33" s="9"/>
       <c r="E33" s="21" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F33" s="22" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="G33" s="21"/>
       <c r="H33" s="18" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="I33" s="18" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="J33" s="18" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="K33" s="18" t="s">
         <v>77</v>
@@ -9283,20 +9300,20 @@
       <c r="C34" s="20"/>
       <c r="D34" s="9"/>
       <c r="E34" s="21" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F34" s="22" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="G34" s="21"/>
       <c r="H34" s="18" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="I34" s="18" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="J34" s="18" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="K34" s="18" t="s">
         <v>77</v>
@@ -9305,7 +9322,7 @@
       <c r="M34" s="18"/>
       <c r="N34" s="18"/>
       <c r="O34" s="18" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="P34" s="18"/>
       <c r="Q34" s="17"/>
@@ -9335,13 +9352,13 @@
         <v>10</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="F35" s="22" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="H35" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="I35" s="0" t="s">
         <v>34</v>
@@ -9354,6 +9371,61 @@
       </c>
       <c r="O35" s="0" t="s">
         <v>37</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="36">
+      <c r="A36" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="E36" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="F36" s="0" t="s">
+        <v>180</v>
+      </c>
+      <c r="H36" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="I36" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="J36" s="0" t="s">
+        <v>182</v>
+      </c>
+      <c r="K36" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="M36" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="O36" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="37">
+      <c r="A37" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="E37" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="F37" s="0" t="s">
+        <v>180</v>
+      </c>
+      <c r="H37" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="I37" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="J37" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="K37" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="O37" s="0" t="s">
+        <v>88</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048574"/>

</xml_diff>

<commit_message>
Compile basic trigger templates
</commit_message>
<xml_diff>
--- a/editor-models/generated-models/src/main/resources/HeD_Templates.xlsx
+++ b/editor-models/generated-models/src/main/resources/HeD_Templates.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="2" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="643" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="643" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Demo Triggers" sheetId="1" state="visible" r:id="rId2"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="183">
   <si>
     <t>Sequence ID</t>
   </si>
@@ -97,226 +97,226 @@
     <t>BaseFrequency</t>
   </si>
   <si>
-    <t>ScheduleAtRelativeTimeFromNow</t>
+    <t>ScheduleAtExactTime</t>
+  </si>
+  <si>
+    <t>TS</t>
+  </si>
+  <si>
+    <t>Act, Trigger</t>
+  </si>
+  <si>
+    <t>UserLogsIn</t>
+  </si>
+  <si>
+    <t>User Event</t>
+  </si>
+  <si>
+    <t>ObservationResult</t>
+  </si>
+  <si>
+    <t>observationFocus</t>
+  </si>
+  <si>
+    <t>codeSystem=TBD;code=login;displayValue=LOGIN</t>
+  </si>
+  <si>
+    <t>CD</t>
+  </si>
+  <si>
+    <t>UserLogsOut</t>
+  </si>
+  <si>
+    <t>codeSystem=TBD;code=logout;displayValue=LOGOUT</t>
+  </si>
+  <si>
+    <t>UserAccessesPatientRecord</t>
+  </si>
+  <si>
+    <t>codeSystem=TBD;code=access;displayValue=ACCESS</t>
+  </si>
+  <si>
+    <t>Update, Trigger</t>
+  </si>
+  <si>
+    <t>PatientInPreadmissionStatus</t>
+  </si>
+  <si>
+    <t>codeSystem=TBD;code=preadmission;displayValue=PREADMIT</t>
+  </si>
+  <si>
+    <t>PatientAdmitted</t>
+  </si>
+  <si>
+    <t>codeSystem=TBD;code=admission;displayValue=ADMIT</t>
+  </si>
+  <si>
+    <t>PatientInPredischargeStatus</t>
+  </si>
+  <si>
+    <t>codeSystem=TBD;code=predischarge;displayValue=PREDISCHARGE</t>
+  </si>
+  <si>
+    <t>PatientDischarged</t>
+  </si>
+  <si>
+    <t>codeSystem=TBD;code=discharge;displayValue=DISCHARGE</t>
+  </si>
+  <si>
+    <t>OutpatientVisit</t>
+  </si>
+  <si>
+    <t>codeSystem=TBD;code=outvisit;displayValue=OUTVISIT</t>
+  </si>
+  <si>
+    <t>LabTestResultAvailable</t>
+  </si>
+  <si>
+    <t>Lab Test Type</t>
+  </si>
+  <si>
+    <t>ProcedureEvent</t>
+  </si>
+  <si>
+    <t>procedureCode</t>
+  </si>
+  <si>
+    <t>1..*</t>
+  </si>
+  <si>
+    <t>codeSystem=LOINC</t>
+  </si>
+  <si>
+    <t>ProcedureResultAvailable</t>
+  </si>
+  <si>
+    <t>Procedure Type</t>
+  </si>
+  <si>
+    <t>codeSystem=SNOMED</t>
+  </si>
+  <si>
+    <t>Findings, Condition</t>
+  </si>
+  <si>
+    <t>PatientAge</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>EvaluatedPerson</t>
+  </si>
+  <si>
+    <t>age</t>
+  </si>
+  <si>
+    <t>unit=years</t>
+  </si>
+  <si>
+    <t>PQ</t>
+  </si>
+  <si>
+    <t>Problem/Diagnosis, Condition</t>
+  </si>
+  <si>
+    <t>ProblemDiagnosis</t>
+  </si>
+  <si>
+    <t>Problem Type</t>
+  </si>
+  <si>
+    <t>Problem</t>
+  </si>
+  <si>
+    <t>problemCode</t>
+  </si>
+  <si>
+    <t>Problem Diagnosed within Date Range</t>
+  </si>
+  <si>
+    <t>diagnosticEventTime</t>
   </si>
   <si>
     <t>unit={days,years,months,hours,minutes,seconds}</t>
   </si>
   <si>
-    <t>PQ</t>
-  </si>
-  <si>
-    <t>ScheduleAtExactTime</t>
-  </si>
-  <si>
-    <t>TS</t>
-  </si>
-  <si>
-    <t>Act, Trigger</t>
-  </si>
-  <si>
-    <t>UserLogsIn</t>
-  </si>
-  <si>
-    <t>User Event</t>
+    <t>Problem Effective within Date Range</t>
+  </si>
+  <si>
+    <t>problemEffectiveTime</t>
+  </si>
+  <si>
+    <t>0..1</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>problemStatus</t>
+  </si>
+  <si>
+    <t>ActiveProblemDiagnosis</t>
+  </si>
+  <si>
+    <t>Date Range</t>
+  </si>
+  <si>
+    <t>codeSystem=TBD;code=active;displayValie=ACTIVE</t>
+  </si>
+  <si>
+    <t>ResolvedProblemDiagnosis</t>
+  </si>
+  <si>
+    <t>codeSystem=TBD;code=resolved;displayValue=RESOLVED</t>
+  </si>
+  <si>
+    <t>StatusPostSurgery</t>
+  </si>
+  <si>
+    <t>Procedure</t>
+  </si>
+  <si>
+    <t>procedureTime</t>
+  </si>
+  <si>
+    <t>IVL_TS</t>
+  </si>
+  <si>
+    <t>Orders/Actions, Condition</t>
+  </si>
+  <si>
+    <t>PatientOnMedication</t>
+  </si>
+  <si>
+    <t>Medication</t>
+  </si>
+  <si>
+    <t>SubstanceAdministrationEvent</t>
+  </si>
+  <si>
+    <t>substanceAdministrationGeneralPurpose</t>
+  </si>
+  <si>
+    <t>codeSystem=RXNORM</t>
+  </si>
+  <si>
+    <t>Last Administration</t>
+  </si>
+  <si>
+    <t>administrationTimeInterval</t>
+  </si>
+  <si>
+    <t>Observations/Results,Condition</t>
+  </si>
+  <si>
+    <t>LabTestResultWithThreshold</t>
+  </si>
+  <si>
+    <t>Observed Quantity</t>
   </si>
   <si>
     <t>Observation</t>
-  </si>
-  <si>
-    <t>observationFocus</t>
-  </si>
-  <si>
-    <t>codeSystem=TBD;code=login;displayValue=LOGIN</t>
-  </si>
-  <si>
-    <t>CD</t>
-  </si>
-  <si>
-    <t>UserLogsOut</t>
-  </si>
-  <si>
-    <t>codeSystem=TBD;code=logout;displayValue=LOGOUT</t>
-  </si>
-  <si>
-    <t>UserAccessesPatientRecord</t>
-  </si>
-  <si>
-    <t>codeSystem=TBD;code=access;displayValue=ACCESS</t>
-  </si>
-  <si>
-    <t>Update, Trigger</t>
-  </si>
-  <si>
-    <t>PatientInPreadmissionStatus</t>
-  </si>
-  <si>
-    <t>codeSystem=TBD;code=preadmission;displayValue=PREADMIT</t>
-  </si>
-  <si>
-    <t>PatientAdmitted</t>
-  </si>
-  <si>
-    <t>codeSystem=TBD;code=admission;displayValue=ADMIT</t>
-  </si>
-  <si>
-    <t>PatientInPredischargeStatus</t>
-  </si>
-  <si>
-    <t>codeSystem=TBD;code=predischarge;displayValue=PREDISCHARGE</t>
-  </si>
-  <si>
-    <t>PatientDischarged</t>
-  </si>
-  <si>
-    <t>codeSystem=TBD;code=discharge;displayValue=DISCHARGE</t>
-  </si>
-  <si>
-    <t>OutpatientVisit</t>
-  </si>
-  <si>
-    <t>codeSystem=TBD;code=outvisit;displayValue=OUTVISIT</t>
-  </si>
-  <si>
-    <t>LabTestResultAvailable</t>
-  </si>
-  <si>
-    <t>Lab Test Type</t>
-  </si>
-  <si>
-    <t>ProcedureEvent</t>
-  </si>
-  <si>
-    <t>procedureCode</t>
-  </si>
-  <si>
-    <t>1..*</t>
-  </si>
-  <si>
-    <t>codeSystem=LOINC</t>
-  </si>
-  <si>
-    <t>ProcedureResultAvailable</t>
-  </si>
-  <si>
-    <t>Procedure Type</t>
-  </si>
-  <si>
-    <t>codeSystem=SNOMED</t>
-  </si>
-  <si>
-    <t>Findings, Condition</t>
-  </si>
-  <si>
-    <t>PatientAge</t>
-  </si>
-  <si>
-    <t>Age</t>
-  </si>
-  <si>
-    <t>EvaluatedPerson</t>
-  </si>
-  <si>
-    <t>age</t>
-  </si>
-  <si>
-    <t>unit=years</t>
-  </si>
-  <si>
-    <t>Problem/Diagnosis, Condition</t>
-  </si>
-  <si>
-    <t>ProblemDiagnosis</t>
-  </si>
-  <si>
-    <t>Problem Type</t>
-  </si>
-  <si>
-    <t>Problem</t>
-  </si>
-  <si>
-    <t>problemCode</t>
-  </si>
-  <si>
-    <t>Problem Diagnosed within Date Range</t>
-  </si>
-  <si>
-    <t>diagnosticEventTime</t>
-  </si>
-  <si>
-    <t>Problem Effective within Date Range</t>
-  </si>
-  <si>
-    <t>problemEffectiveTime</t>
-  </si>
-  <si>
-    <t>0..1</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>problemStatus</t>
-  </si>
-  <si>
-    <t>ActiveProblemDiagnosis</t>
-  </si>
-  <si>
-    <t>Date Range</t>
-  </si>
-  <si>
-    <t>codeSystem=TBD;code=active;displayValie=ACTIVE</t>
-  </si>
-  <si>
-    <t>ResolvedProblemDiagnosis</t>
-  </si>
-  <si>
-    <t>codeSystem=TBD;code=resolved;displayValue=RESOLVED</t>
-  </si>
-  <si>
-    <t>StatusPostSurgery</t>
-  </si>
-  <si>
-    <t>Procedure</t>
-  </si>
-  <si>
-    <t>procedureTime</t>
-  </si>
-  <si>
-    <t>IVL_TS</t>
-  </si>
-  <si>
-    <t>Orders/Actions, Condition</t>
-  </si>
-  <si>
-    <t>PatientOnMedication</t>
-  </si>
-  <si>
-    <t>Medication</t>
-  </si>
-  <si>
-    <t>SubstanceAdministrationEvent</t>
-  </si>
-  <si>
-    <t>substanceAdministrationGeneralPurpose</t>
-  </si>
-  <si>
-    <t>codeSystem=RXNORM</t>
-  </si>
-  <si>
-    <t>Last Administration</t>
-  </si>
-  <si>
-    <t>administrationTimeInterval</t>
-  </si>
-  <si>
-    <t>Observations/Results,Condition</t>
-  </si>
-  <si>
-    <t>LabTestResultWithThreshold</t>
-  </si>
-  <si>
-    <t>Observed Quantity</t>
   </si>
   <si>
     <t>Threshold</t>
@@ -870,8 +870,8 @@
   </sheetPr>
   <dimension ref="A1:R14"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A14" activeCellId="0" pane="topLeft" sqref="A14"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="D1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="D3" activeCellId="0" pane="topLeft" sqref="3:3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -972,41 +972,15 @@
         <v>25</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="3">
-      <c r="A3" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="H3" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="I3" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="J3" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="K3" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="M3" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="O3" s="0" t="s">
-        <v>28</v>
-      </c>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="3">
+      <c r="F3" s="7"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="4">
       <c r="E4" s="0" t="s">
         <v>19</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="H4" s="0" t="s">
         <v>21</v>
@@ -1021,7 +995,7 @@
         <v>24</v>
       </c>
       <c r="O4" s="0" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="5">
@@ -1029,28 +1003,28 @@
         <v>3</v>
       </c>
       <c r="E5" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="I5" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="F5" s="0" t="s">
+      <c r="J5" s="0" t="s">
         <v>32</v>
-      </c>
-      <c r="H5" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="I5" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="J5" s="0" t="s">
-        <v>35</v>
       </c>
       <c r="K5" s="0" t="s">
         <v>24</v>
       </c>
       <c r="M5" s="0" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="O5" s="0" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="6">
@@ -1058,28 +1032,28 @@
         <v>4</v>
       </c>
       <c r="E6" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="I6" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="F6" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="H6" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="I6" s="0" t="s">
-        <v>34</v>
-      </c>
       <c r="J6" s="0" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="K6" s="0" t="s">
         <v>24</v>
       </c>
       <c r="M6" s="0" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="O6" s="0" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="7">
@@ -1087,28 +1061,28 @@
         <v>5</v>
       </c>
       <c r="E7" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="H7" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="I7" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="F7" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="H7" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="I7" s="0" t="s">
-        <v>34</v>
-      </c>
       <c r="J7" s="0" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="K7" s="0" t="s">
         <v>24</v>
       </c>
       <c r="M7" s="0" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="O7" s="0" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="8">
@@ -1116,28 +1090,28 @@
         <v>6</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="J8" s="0" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="K8" s="0" t="s">
         <v>24</v>
       </c>
       <c r="M8" s="0" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="O8" s="0" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="9">
@@ -1145,28 +1119,28 @@
         <v>7</v>
       </c>
       <c r="E9" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="F9" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="F9" s="0" t="s">
-        <v>45</v>
-      </c>
       <c r="H9" s="0" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="J9" s="0" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="K9" s="0" t="s">
         <v>24</v>
       </c>
       <c r="M9" s="0" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="O9" s="0" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="10">
@@ -1174,28 +1148,28 @@
         <v>8</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="J10" s="0" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="K10" s="0" t="s">
         <v>24</v>
       </c>
       <c r="M10" s="0" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="O10" s="0" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="11">
@@ -1203,28 +1177,28 @@
         <v>9</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="I11" s="0" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="J11" s="0" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="K11" s="0" t="s">
         <v>24</v>
       </c>
       <c r="M11" s="0" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="O11" s="0" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="12">
@@ -1232,28 +1206,28 @@
         <v>10</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="I12" s="0" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="J12" s="0" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="K12" s="0" t="s">
         <v>24</v>
       </c>
       <c r="M12" s="0" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="O12" s="0" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="13">
@@ -1261,28 +1235,28 @@
         <v>11</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F13" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="H13" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="I13" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="J13" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="H13" s="0" t="s">
+      <c r="K13" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="I13" s="0" t="s">
+      <c r="M13" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="J13" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="K13" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="M13" s="0" t="s">
-        <v>58</v>
-      </c>
       <c r="O13" s="0" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="14">
@@ -1290,28 +1264,28 @@
         <v>12</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="I14" s="0" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="J14" s="0" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="K14" s="0" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="M14" s="0" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="O14" s="0" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1333,7 +1307,7 @@
   <dimension ref="A1:R49"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A34" activeCellId="0" pane="topLeft" sqref="A34"/>
+      <selection activeCell="A34" activeCellId="1" pane="topLeft" sqref="3:3 A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.1"/>
@@ -1414,31 +1388,31 @@
       <c r="C2" s="8"/>
       <c r="D2" s="9"/>
       <c r="E2" s="8" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="G2" s="8"/>
       <c r="H2" s="10" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="K2" s="8" t="s">
         <v>24</v>
       </c>
       <c r="L2" s="8"/>
       <c r="M2" s="11" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="N2" s="11"/>
       <c r="O2" s="10" t="s">
-        <v>28</v>
+        <v>65</v>
       </c>
       <c r="P2" s="10"/>
       <c r="Q2" s="8"/>
@@ -1469,28 +1443,28 @@
         <v>1</v>
       </c>
       <c r="E4" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="H4" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="F4" s="0" t="s">
+      <c r="I4" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="H4" s="0" t="s">
+      <c r="J4" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="I4" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="J4" s="0" t="s">
-        <v>72</v>
-      </c>
       <c r="K4" s="0" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="M4" s="0" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="O4" s="0" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="5">
@@ -1498,28 +1472,28 @@
         <v>1</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F5" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="I5" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="H5" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="I5" s="0" t="s">
-        <v>71</v>
-      </c>
       <c r="J5" s="0" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="K5" s="0" t="s">
         <v>24</v>
       </c>
       <c r="M5" s="0" t="s">
-        <v>27</v>
+        <v>73</v>
       </c>
       <c r="O5" s="0" t="s">
-        <v>28</v>
+        <v>65</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="6">
@@ -1527,28 +1501,28 @@
         <v>1</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F6" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="I6" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="H6" s="0" t="s">
+      <c r="J6" s="0" t="s">
         <v>75</v>
       </c>
-      <c r="I6" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="J6" s="0" t="s">
+      <c r="K6" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="K6" s="0" t="s">
-        <v>77</v>
-      </c>
       <c r="M6" s="0" t="s">
-        <v>27</v>
+        <v>73</v>
       </c>
       <c r="O6" s="0" t="s">
-        <v>28</v>
+        <v>65</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="7">
@@ -1556,25 +1530,25 @@
         <v>1</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F7" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="H7" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="I7" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="H7" s="0" t="s">
+      <c r="J7" s="0" t="s">
         <v>78</v>
-      </c>
-      <c r="I7" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="J7" s="0" t="s">
-        <v>79</v>
       </c>
       <c r="K7" s="0" t="s">
         <v>24</v>
       </c>
       <c r="O7" s="0" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="9">
@@ -1582,28 +1556,28 @@
         <v>2</v>
       </c>
       <c r="E9" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="H9" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="F9" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="H9" s="0" t="s">
+      <c r="I9" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="J9" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="I9" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="J9" s="0" t="s">
-        <v>72</v>
-      </c>
       <c r="K9" s="0" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="M9" s="0" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="O9" s="0" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="10">
@@ -1611,28 +1585,28 @@
         <v>2</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="J10" s="0" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="K10" s="0" t="s">
         <v>24</v>
       </c>
       <c r="M10" s="0" t="s">
-        <v>27</v>
+        <v>73</v>
       </c>
       <c r="O10" s="0" t="s">
-        <v>28</v>
+        <v>65</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="11">
@@ -1640,25 +1614,25 @@
         <v>2</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F11" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="H11" s="0" t="s">
         <v>80</v>
       </c>
-      <c r="H11" s="0" t="s">
-        <v>81</v>
-      </c>
       <c r="I11" s="0" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="J11" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="K11" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="K11" s="0" t="s">
-        <v>77</v>
-      </c>
       <c r="O11" s="0" t="s">
-        <v>28</v>
+        <v>65</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="12">
@@ -1666,28 +1640,28 @@
         <v>2</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H12" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="I12" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="J12" s="0" t="s">
         <v>78</v>
-      </c>
-      <c r="I12" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="J12" s="0" t="s">
-        <v>79</v>
       </c>
       <c r="K12" s="0" t="s">
         <v>24</v>
       </c>
       <c r="M12" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="O12" s="0" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="14">
@@ -1695,28 +1669,28 @@
         <v>3</v>
       </c>
       <c r="E14" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="F14" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="H14" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="F14" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="H14" s="0" t="s">
+      <c r="I14" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="J14" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="I14" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="J14" s="0" t="s">
-        <v>72</v>
-      </c>
       <c r="K14" s="0" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="M14" s="0" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="O14" s="0" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="15">
@@ -1724,28 +1698,28 @@
         <v>3</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="I15" s="0" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="J15" s="0" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="K15" s="0" t="s">
         <v>24</v>
       </c>
       <c r="M15" s="0" t="s">
-        <v>27</v>
+        <v>73</v>
       </c>
       <c r="O15" s="0" t="s">
-        <v>28</v>
+        <v>65</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="16">
@@ -1753,25 +1727,25 @@
         <v>3</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I16" s="0" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="J16" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="K16" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="K16" s="0" t="s">
-        <v>77</v>
-      </c>
       <c r="O16" s="0" t="s">
-        <v>28</v>
+        <v>65</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="17">
@@ -1779,28 +1753,28 @@
         <v>3</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H17" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="I17" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="J17" s="0" t="s">
         <v>78</v>
-      </c>
-      <c r="I17" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="J17" s="0" t="s">
-        <v>79</v>
       </c>
       <c r="K17" s="0" t="s">
         <v>24</v>
       </c>
       <c r="M17" s="0" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="O17" s="0" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="20">
@@ -1808,28 +1782,28 @@
         <v>20</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F20" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="H20" s="0" t="s">
         <v>85</v>
       </c>
-      <c r="H20" s="0" t="s">
-        <v>86</v>
-      </c>
       <c r="I20" s="0" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="J20" s="0" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="K20" s="0" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="M20" s="0" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="O20" s="0" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="21">
@@ -1837,25 +1811,25 @@
         <v>20</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H21" s="0" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I21" s="0" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="J21" s="0" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K21" s="0" t="s">
         <v>24</v>
       </c>
       <c r="O21" s="0" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="23">
@@ -1863,28 +1837,28 @@
         <v>30</v>
       </c>
       <c r="E23" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="F23" s="0" t="s">
         <v>89</v>
       </c>
-      <c r="F23" s="0" t="s">
+      <c r="H23" s="0" t="s">
         <v>90</v>
       </c>
-      <c r="H23" s="0" t="s">
+      <c r="I23" s="0" t="s">
         <v>91</v>
       </c>
-      <c r="I23" s="0" t="s">
+      <c r="J23" s="0" t="s">
         <v>92</v>
       </c>
-      <c r="J23" s="0" t="s">
+      <c r="K23" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="M23" s="0" t="s">
         <v>93</v>
       </c>
-      <c r="K23" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="M23" s="0" t="s">
-        <v>94</v>
-      </c>
       <c r="O23" s="0" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="24">
@@ -1892,25 +1866,25 @@
         <v>30</v>
       </c>
       <c r="E24" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="F24" s="0" t="s">
         <v>89</v>
       </c>
-      <c r="F24" s="0" t="s">
-        <v>90</v>
-      </c>
       <c r="H24" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="I24" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="J24" s="0" t="s">
         <v>95</v>
-      </c>
-      <c r="I24" s="0" t="s">
-        <v>92</v>
-      </c>
-      <c r="J24" s="0" t="s">
-        <v>96</v>
       </c>
       <c r="K24" s="0" t="s">
         <v>24</v>
       </c>
       <c r="O24" s="0" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="25">
@@ -1918,28 +1892,28 @@
         <v>40</v>
       </c>
       <c r="E25" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="F25" s="0" t="s">
         <v>97</v>
       </c>
-      <c r="F25" s="0" t="s">
+      <c r="H25" s="0" t="s">
         <v>98</v>
       </c>
-      <c r="H25" s="0" t="s">
+      <c r="I25" s="0" t="s">
         <v>99</v>
       </c>
-      <c r="I25" s="0" t="s">
-        <v>34</v>
-      </c>
       <c r="J25" s="0" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="K25" s="0" t="s">
         <v>24</v>
       </c>
       <c r="M25" s="0" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="O25" s="0" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="26">
@@ -1947,16 +1921,16 @@
         <v>40</v>
       </c>
       <c r="E26" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="F26" s="0" t="s">
         <v>97</v>
-      </c>
-      <c r="F26" s="0" t="s">
-        <v>98</v>
       </c>
       <c r="H26" s="0" t="s">
         <v>100</v>
       </c>
       <c r="I26" s="0" t="s">
-        <v>34</v>
+        <v>99</v>
       </c>
       <c r="J26" s="0" t="s">
         <v>101</v>
@@ -1965,7 +1939,7 @@
         <v>24</v>
       </c>
       <c r="O26" s="0" t="s">
-        <v>28</v>
+        <v>65</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="28">
@@ -1982,19 +1956,19 @@
         <v>104</v>
       </c>
       <c r="I28" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="J28" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="K28" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="M28" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="J28" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="K28" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="M28" s="0" t="s">
-        <v>58</v>
-      </c>
       <c r="O28" s="0" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="23.85" outlineLevel="0" r="29">
@@ -2011,19 +1985,19 @@
         <v>105</v>
       </c>
       <c r="I29" s="0" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="J29" s="0" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K29" s="0" t="s">
         <v>24</v>
       </c>
       <c r="M29" s="15" t="s">
-        <v>27</v>
+        <v>73</v>
       </c>
       <c r="O29" s="0" t="s">
-        <v>28</v>
+        <v>65</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="30">
@@ -2045,19 +2019,19 @@
         <v>104</v>
       </c>
       <c r="I31" s="0" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="J31" s="0" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="K31" s="0" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="M31" s="0" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="O31" s="0" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="23.85" outlineLevel="0" r="32">
@@ -2074,19 +2048,19 @@
         <v>105</v>
       </c>
       <c r="I32" s="0" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="J32" s="0" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K32" s="0" t="s">
         <v>24</v>
       </c>
       <c r="M32" s="15" t="s">
-        <v>27</v>
+        <v>73</v>
       </c>
       <c r="O32" s="0" t="s">
-        <v>28</v>
+        <v>65</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="47">
@@ -2097,7 +2071,7 @@
         <v>18</v>
       </c>
       <c r="E47" s="0" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F47" s="0" t="s">
         <v>107</v>
@@ -2106,19 +2080,19 @@
         <v>108</v>
       </c>
       <c r="I47" s="0" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="J47" s="0" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="K47" s="0" t="s">
         <v>24</v>
       </c>
       <c r="M47" s="0" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="O47" s="0" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="P47" s="0" t="s">
         <v>109</v>
@@ -2129,25 +2103,25 @@
         <v>99</v>
       </c>
       <c r="E48" s="0" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F48" s="0" t="s">
         <v>107</v>
       </c>
       <c r="H48" s="0" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I48" s="0" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="J48" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="K48" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="K48" s="0" t="s">
-        <v>77</v>
-      </c>
       <c r="O48" s="0" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="49">
@@ -2155,19 +2129,19 @@
         <v>99</v>
       </c>
       <c r="E49" s="0" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F49" s="0" t="s">
         <v>107</v>
       </c>
       <c r="H49" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="I49" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="J49" s="0" t="s">
         <v>78</v>
-      </c>
-      <c r="I49" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="J49" s="0" t="s">
-        <v>79</v>
       </c>
       <c r="K49" s="0" t="s">
         <v>24</v>
@@ -2176,7 +2150,7 @@
         <v>110</v>
       </c>
       <c r="O49" s="0" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -2197,8 +2171,8 @@
   </sheetPr>
   <dimension ref="A1:ALZ65536"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A38" activeCellId="0" pane="topLeft" sqref="A38"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="G1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="I36" activeCellId="1" pane="topLeft" sqref="3:3 I36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.1"/>
@@ -2741,10 +2715,10 @@
         <v>118</v>
       </c>
       <c r="K3" s="18" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="O3" s="18" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="Q3" s="17"/>
       <c r="R3" s="17"/>
@@ -3202,10 +3176,10 @@
         <v>120</v>
       </c>
       <c r="K4" s="18" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="O4" s="18" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="Q4" s="17"/>
       <c r="R4" s="17"/>
@@ -3663,10 +3637,10 @@
         <v>122</v>
       </c>
       <c r="K5" s="18" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="O5" s="18" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="Q5" s="17"/>
       <c r="R5" s="17"/>
@@ -4124,7 +4098,7 @@
         <v>124</v>
       </c>
       <c r="K6" s="18" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="O6" s="18" t="s">
         <v>125</v>
@@ -4585,7 +4559,7 @@
         <v>127</v>
       </c>
       <c r="K7" s="18" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="O7" s="18" t="s">
         <v>128</v>
@@ -5046,7 +5020,7 @@
         <v>130</v>
       </c>
       <c r="K8" s="18" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="O8" s="18" t="s">
         <v>131</v>
@@ -5507,7 +5481,7 @@
         <v>133</v>
       </c>
       <c r="K9" s="18" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="O9" s="18" t="s">
         <v>134</v>
@@ -5968,7 +5942,7 @@
         <v>136</v>
       </c>
       <c r="K10" s="18" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="O10" s="18" t="s">
         <v>125</v>
@@ -6429,7 +6403,7 @@
         <v>138</v>
       </c>
       <c r="K11" s="18" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="O11" s="18" t="s">
         <v>128</v>
@@ -6890,7 +6864,7 @@
         <v>140</v>
       </c>
       <c r="K12" s="18" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="O12" s="18" t="s">
         <v>131</v>
@@ -7351,7 +7325,7 @@
         <v>142</v>
       </c>
       <c r="K13" s="18" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="O13" s="18" t="s">
         <v>134</v>
@@ -7812,10 +7786,10 @@
         <v>144</v>
       </c>
       <c r="K14" s="18" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="O14" s="18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="Q14" s="17"/>
       <c r="R14" s="17"/>
@@ -8274,13 +8248,13 @@
         <v>149</v>
       </c>
       <c r="K15" s="18" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="L15" s="18"/>
       <c r="M15" s="18"/>
       <c r="N15" s="18"/>
       <c r="O15" s="18" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="P15" s="18"/>
       <c r="Q15" s="22"/>
@@ -8329,13 +8303,13 @@
         <v>151</v>
       </c>
       <c r="K16" s="18" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="L16" s="18"/>
       <c r="M16" s="18"/>
       <c r="N16" s="18"/>
       <c r="O16" s="18" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="P16" s="18"/>
       <c r="Q16" s="17"/>
@@ -8384,13 +8358,13 @@
         <v>153</v>
       </c>
       <c r="K17" s="18" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="L17" s="18"/>
       <c r="M17" s="18"/>
       <c r="N17" s="18"/>
       <c r="O17" s="18" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="P17" s="18"/>
       <c r="Q17" s="17"/>
@@ -8439,13 +8413,13 @@
         <v>155</v>
       </c>
       <c r="K18" s="18" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="L18" s="18"/>
       <c r="M18" s="18"/>
       <c r="N18" s="18"/>
       <c r="O18" s="18" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="P18" s="18"/>
       <c r="Q18" s="17"/>
@@ -8494,7 +8468,7 @@
         <v>157</v>
       </c>
       <c r="K19" s="18" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="L19" s="18"/>
       <c r="M19" s="18"/>
@@ -8546,16 +8520,16 @@
         <v>148</v>
       </c>
       <c r="J20" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K20" s="18" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="L20" s="18"/>
       <c r="M20" s="18"/>
       <c r="N20" s="18"/>
       <c r="O20" s="18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="P20" s="18"/>
       <c r="Q20" s="17"/>
@@ -8604,13 +8578,13 @@
         <v>161</v>
       </c>
       <c r="K21" s="18" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="L21" s="18"/>
       <c r="M21" s="18"/>
       <c r="N21" s="18"/>
       <c r="O21" s="18" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="P21" s="18"/>
       <c r="R21" s="17"/>
@@ -8658,7 +8632,7 @@
         <v>163</v>
       </c>
       <c r="K22" s="18" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="L22" s="18"/>
       <c r="M22" s="18"/>
@@ -8713,7 +8687,7 @@
         <v>166</v>
       </c>
       <c r="K23" s="18" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="L23" s="18"/>
       <c r="M23" s="18"/>
@@ -8768,7 +8742,7 @@
         <v>23</v>
       </c>
       <c r="K24" s="18" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="L24" s="18"/>
       <c r="M24" s="18"/>
@@ -8823,13 +8797,13 @@
         <v>168</v>
       </c>
       <c r="K25" s="18" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="L25" s="18"/>
       <c r="M25" s="18"/>
       <c r="N25" s="18"/>
       <c r="O25" s="18" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="P25" s="18"/>
       <c r="Q25" s="17"/>
@@ -8878,7 +8852,7 @@
         <v>170</v>
       </c>
       <c r="K26" s="18" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="L26" s="18"/>
       <c r="M26" s="18"/>
@@ -8933,13 +8907,13 @@
         <v>149</v>
       </c>
       <c r="K27" s="18" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="L27" s="18"/>
       <c r="M27" s="18"/>
       <c r="N27" s="18"/>
       <c r="O27" s="18" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="P27" s="18"/>
       <c r="Q27" s="17"/>
@@ -8988,13 +8962,13 @@
         <v>155</v>
       </c>
       <c r="K28" s="21" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="L28" s="21"/>
       <c r="M28" s="21"/>
       <c r="N28" s="21"/>
       <c r="O28" s="21" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="P28" s="21"/>
       <c r="Q28" s="22"/>
@@ -9043,13 +9017,13 @@
         <v>175</v>
       </c>
       <c r="K29" s="18" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="L29" s="18"/>
       <c r="M29" s="18"/>
       <c r="N29" s="18"/>
       <c r="O29" s="18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="P29" s="18"/>
       <c r="Q29" s="17"/>
@@ -9098,13 +9072,13 @@
         <v>161</v>
       </c>
       <c r="K30" s="17" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="L30" s="17"/>
       <c r="M30" s="17"/>
       <c r="N30" s="17"/>
       <c r="O30" s="17" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="P30" s="17"/>
       <c r="Q30" s="17"/>
@@ -9152,7 +9126,7 @@
         <v>163</v>
       </c>
       <c r="K31" s="18" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="L31" s="18"/>
       <c r="M31" s="18"/>
@@ -9207,7 +9181,7 @@
         <v>166</v>
       </c>
       <c r="K32" s="18" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="L32" s="18"/>
       <c r="M32" s="18"/>
@@ -9262,13 +9236,13 @@
         <v>168</v>
       </c>
       <c r="K33" s="18" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="L33" s="18"/>
       <c r="M33" s="18"/>
       <c r="N33" s="18"/>
       <c r="O33" s="18" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="P33" s="18"/>
       <c r="Q33" s="17"/>
@@ -9316,7 +9290,7 @@
         <v>170</v>
       </c>
       <c r="K34" s="18" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="L34" s="18"/>
       <c r="M34" s="18"/>
@@ -9361,7 +9335,7 @@
         <v>179</v>
       </c>
       <c r="I35" s="0" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="J35" s="0" t="s">
         <v>101</v>
@@ -9370,7 +9344,7 @@
         <v>24</v>
       </c>
       <c r="O35" s="0" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="36">
@@ -9387,7 +9361,7 @@
         <v>181</v>
       </c>
       <c r="I36" s="0" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J36" s="0" t="s">
         <v>182</v>
@@ -9396,10 +9370,10 @@
         <v>24</v>
       </c>
       <c r="M36" s="0" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="O36" s="0" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="37">
@@ -9416,16 +9390,16 @@
         <v>159</v>
       </c>
       <c r="I37" s="0" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J37" s="0" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K37" s="0" t="s">
         <v>24</v>
       </c>
       <c r="O37" s="0" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048574"/>

</xml_diff>

<commit_message>
Various UI fixes, template instantiation, misc
</commit_message>
<xml_diff>
--- a/editor-models/generated-models/src/main/resources/HeD_Templates.xlsx
+++ b/editor-models/generated-models/src/main/resources/HeD_Templates.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="643" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="1" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="643" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Demo Triggers" sheetId="1" state="visible" r:id="rId2"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="181">
   <si>
     <t>Sequence ID</t>
   </si>
@@ -79,7 +79,7 @@
     <t>Timed, Trigger</t>
   </si>
   <si>
-    <t>ScheduleAtRecurringTime</t>
+    <t>RecurringTimeEvent</t>
   </si>
   <si>
     <t>At Time</t>
@@ -97,7 +97,7 @@
     <t>BaseFrequency</t>
   </si>
   <si>
-    <t>ScheduleAtExactTime</t>
+    <t>SpecificTimeEvent</t>
   </si>
   <si>
     <t>TS</t>
@@ -316,18 +316,12 @@
     <t>Observed Quantity</t>
   </si>
   <si>
-    <t>Observation</t>
-  </si>
-  <si>
     <t>Threshold</t>
   </si>
   <si>
     <t>observationValue</t>
   </si>
   <si>
-    <t>Procedures, Condition</t>
-  </si>
-  <si>
     <t>LabTestWithinTimeInterval</t>
   </si>
   <si>
@@ -535,7 +529,7 @@
     <t>INT</t>
   </si>
   <si>
-    <t>MedicationOrderProposal</t>
+    <t>MedicationOrderReccomendation</t>
   </si>
   <si>
     <t>SubstanceAdministrationProposal/</t>
@@ -559,13 +553,13 @@
     <t>Concept</t>
   </si>
   <si>
-    <t>MedicationIntake</t>
+    <t>MedicationAdministration</t>
   </si>
   <si>
     <t>Drug Taken</t>
   </si>
   <si>
-    <t>substance</t>
+    <t>substanceCode</t>
   </si>
 </sst>
 </file>
@@ -581,7 +575,6 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -604,14 +597,12 @@
       <color rgb="FF000000"/>
       <name val="Verdana"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="8"/>
       <color rgb="FF000000"/>
       <name val="Verdana"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <strike val="true"/>
@@ -619,7 +610,6 @@
       <color rgb="FF000000"/>
       <name val="Verdana"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="7">
@@ -870,8 +860,8 @@
   </sheetPr>
   <dimension ref="A1:R14"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="D1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="D3" activeCellId="0" pane="topLeft" sqref="3:3"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="D1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="F5" activeCellId="0" pane="topLeft" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1306,8 +1296,8 @@
   </sheetPr>
   <dimension ref="A1:R49"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A34" activeCellId="1" pane="topLeft" sqref="3:3 A34"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="F37" activeCellId="0" pane="topLeft" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.1"/>
@@ -1317,7 +1307,7 @@
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.4183673469388"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.5204081632653"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="27.780612244898"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.6122448979592"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="27.780612244898"/>
     <col collapsed="false" hidden="false" max="12" min="11" style="0" width="11.5204081632653"/>
     <col collapsed="false" hidden="false" max="13" min="13" style="0" width="29.8673469387755"/>
@@ -1901,7 +1891,7 @@
         <v>98</v>
       </c>
       <c r="I25" s="0" t="s">
-        <v>99</v>
+        <v>31</v>
       </c>
       <c r="J25" s="0" t="s">
         <v>32</v>
@@ -1927,13 +1917,13 @@
         <v>97</v>
       </c>
       <c r="H26" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="I26" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="J26" s="0" t="s">
         <v>100</v>
-      </c>
-      <c r="I26" s="0" t="s">
-        <v>99</v>
-      </c>
-      <c r="J26" s="0" t="s">
-        <v>101</v>
       </c>
       <c r="K26" s="0" t="s">
         <v>24</v>
@@ -1947,13 +1937,13 @@
         <v>50</v>
       </c>
       <c r="E28" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="F28" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="H28" s="0" t="s">
         <v>102</v>
-      </c>
-      <c r="F28" s="0" t="s">
-        <v>103</v>
-      </c>
-      <c r="H28" s="0" t="s">
-        <v>104</v>
       </c>
       <c r="I28" s="0" t="s">
         <v>52</v>
@@ -1976,13 +1966,13 @@
         <v>50</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="F29" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="H29" s="0" t="s">
         <v>103</v>
-      </c>
-      <c r="H29" s="0" t="s">
-        <v>105</v>
       </c>
       <c r="I29" s="0" t="s">
         <v>52</v>
@@ -2002,7 +1992,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="30">
       <c r="E30" s="0" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="31">
@@ -2010,13 +2000,13 @@
         <v>60</v>
       </c>
       <c r="E31" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="F31" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="H31" s="0" t="s">
         <v>102</v>
-      </c>
-      <c r="F31" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="H31" s="0" t="s">
-        <v>104</v>
       </c>
       <c r="I31" s="0" t="s">
         <v>52</v>
@@ -2039,13 +2029,13 @@
         <v>60</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="H32" s="0" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="I32" s="0" t="s">
         <v>52</v>
@@ -2074,10 +2064,10 @@
         <v>66</v>
       </c>
       <c r="F47" s="0" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="H47" s="0" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="I47" s="0" t="s">
         <v>69</v>
@@ -2095,7 +2085,7 @@
         <v>34</v>
       </c>
       <c r="P47" s="0" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="48">
@@ -2106,7 +2096,7 @@
         <v>66</v>
       </c>
       <c r="F48" s="0" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="H48" s="0" t="s">
         <v>80</v>
@@ -2132,7 +2122,7 @@
         <v>66</v>
       </c>
       <c r="F49" s="0" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="H49" s="0" t="s">
         <v>77</v>
@@ -2147,7 +2137,7 @@
         <v>24</v>
       </c>
       <c r="M49" s="0" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="O49" s="0" t="s">
         <v>34</v>
@@ -2171,8 +2161,8 @@
   </sheetPr>
   <dimension ref="A1:ALZ65536"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="G1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="I36" activeCellId="1" pane="topLeft" sqref="3:3 I36"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="F43" activeCellId="0" pane="topLeft" sqref="F43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.1"/>
@@ -2239,25 +2229,25 @@
       <c r="C2" s="17"/>
       <c r="D2" s="17"/>
       <c r="E2" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="H2" s="18" t="s">
         <v>111</v>
       </c>
-      <c r="F2" s="17" t="s">
+      <c r="I2" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="H2" s="18" t="s">
+      <c r="J2" s="18" t="s">
         <v>113</v>
-      </c>
-      <c r="I2" s="18" t="s">
-        <v>114</v>
-      </c>
-      <c r="J2" s="18" t="s">
-        <v>115</v>
       </c>
       <c r="K2" s="18" t="s">
         <v>24</v>
       </c>
       <c r="O2" s="18" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="Q2" s="17"/>
       <c r="R2" s="17"/>
@@ -2700,19 +2690,19 @@
       <c r="C3" s="17"/>
       <c r="D3" s="17"/>
       <c r="E3" s="18" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F3" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="H3" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="I3" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="H3" s="18" t="s">
-        <v>117</v>
-      </c>
-      <c r="I3" s="18" t="s">
-        <v>114</v>
-      </c>
       <c r="J3" s="18" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="K3" s="18" t="s">
         <v>76</v>
@@ -3161,19 +3151,19 @@
       <c r="C4" s="17"/>
       <c r="D4" s="17"/>
       <c r="E4" s="18" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F4" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="H4" s="18" t="s">
+        <v>117</v>
+      </c>
+      <c r="I4" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="H4" s="18" t="s">
-        <v>119</v>
-      </c>
-      <c r="I4" s="18" t="s">
-        <v>114</v>
-      </c>
       <c r="J4" s="18" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="K4" s="18" t="s">
         <v>76</v>
@@ -3622,19 +3612,19 @@
       <c r="C5" s="17"/>
       <c r="D5" s="17"/>
       <c r="E5" s="18" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F5" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="H5" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="I5" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="H5" s="18" t="s">
-        <v>121</v>
-      </c>
-      <c r="I5" s="18" t="s">
-        <v>114</v>
-      </c>
       <c r="J5" s="18" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="K5" s="18" t="s">
         <v>76</v>
@@ -4083,25 +4073,25 @@
       <c r="C6" s="17"/>
       <c r="D6" s="17"/>
       <c r="E6" s="18" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F6" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="H6" s="18" t="s">
+        <v>121</v>
+      </c>
+      <c r="I6" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="H6" s="18" t="s">
-        <v>123</v>
-      </c>
-      <c r="I6" s="18" t="s">
-        <v>114</v>
-      </c>
       <c r="J6" s="18" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="K6" s="18" t="s">
         <v>76</v>
       </c>
       <c r="O6" s="18" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="Q6" s="17"/>
       <c r="R6" s="17"/>
@@ -4544,25 +4534,25 @@
       <c r="C7" s="17"/>
       <c r="D7" s="17"/>
       <c r="E7" s="18" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F7" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="H7" s="18" t="s">
+        <v>124</v>
+      </c>
+      <c r="I7" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="H7" s="18" t="s">
-        <v>126</v>
-      </c>
-      <c r="I7" s="18" t="s">
-        <v>114</v>
-      </c>
       <c r="J7" s="18" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="K7" s="18" t="s">
         <v>76</v>
       </c>
       <c r="O7" s="18" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="Q7" s="17"/>
       <c r="R7" s="17"/>
@@ -5005,25 +4995,25 @@
       <c r="C8" s="17"/>
       <c r="D8" s="17"/>
       <c r="E8" s="18" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F8" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="H8" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="I8" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="H8" s="18" t="s">
-        <v>129</v>
-      </c>
-      <c r="I8" s="18" t="s">
-        <v>114</v>
-      </c>
       <c r="J8" s="18" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="K8" s="18" t="s">
         <v>76</v>
       </c>
       <c r="O8" s="18" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="Q8" s="17"/>
       <c r="R8" s="17"/>
@@ -5466,25 +5456,25 @@
       <c r="C9" s="17"/>
       <c r="D9" s="17"/>
       <c r="E9" s="18" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F9" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="H9" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="I9" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="H9" s="18" t="s">
-        <v>132</v>
-      </c>
-      <c r="I9" s="18" t="s">
-        <v>114</v>
-      </c>
       <c r="J9" s="18" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="K9" s="18" t="s">
         <v>76</v>
       </c>
       <c r="O9" s="18" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="Q9" s="17"/>
       <c r="R9" s="17"/>
@@ -5927,25 +5917,25 @@
       <c r="C10" s="17"/>
       <c r="D10" s="17"/>
       <c r="E10" s="18" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F10" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="H10" s="18" t="s">
+        <v>133</v>
+      </c>
+      <c r="I10" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="H10" s="18" t="s">
-        <v>135</v>
-      </c>
-      <c r="I10" s="18" t="s">
-        <v>114</v>
-      </c>
       <c r="J10" s="18" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="K10" s="18" t="s">
         <v>76</v>
       </c>
       <c r="O10" s="18" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="Q10" s="17"/>
       <c r="R10" s="17"/>
@@ -6388,25 +6378,25 @@
       <c r="C11" s="17"/>
       <c r="D11" s="17"/>
       <c r="E11" s="18" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F11" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="H11" s="18" t="s">
+        <v>135</v>
+      </c>
+      <c r="I11" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="H11" s="18" t="s">
-        <v>137</v>
-      </c>
-      <c r="I11" s="18" t="s">
-        <v>114</v>
-      </c>
       <c r="J11" s="18" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="K11" s="18" t="s">
         <v>76</v>
       </c>
       <c r="O11" s="18" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="Q11" s="17"/>
       <c r="R11" s="17"/>
@@ -6849,25 +6839,25 @@
       <c r="C12" s="17"/>
       <c r="D12" s="17"/>
       <c r="E12" s="18" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F12" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="H12" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="I12" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="H12" s="18" t="s">
-        <v>139</v>
-      </c>
-      <c r="I12" s="18" t="s">
-        <v>114</v>
-      </c>
       <c r="J12" s="18" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="K12" s="18" t="s">
         <v>76</v>
       </c>
       <c r="O12" s="18" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="Q12" s="17"/>
       <c r="R12" s="17"/>
@@ -7310,25 +7300,25 @@
       <c r="C13" s="17"/>
       <c r="D13" s="17"/>
       <c r="E13" s="18" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F13" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="H13" s="18" t="s">
+        <v>139</v>
+      </c>
+      <c r="I13" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="H13" s="18" t="s">
-        <v>141</v>
-      </c>
-      <c r="I13" s="18" t="s">
-        <v>114</v>
-      </c>
       <c r="J13" s="18" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="K13" s="18" t="s">
         <v>76</v>
       </c>
       <c r="O13" s="18" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="Q13" s="17"/>
       <c r="R13" s="17"/>
@@ -7771,19 +7761,19 @@
       <c r="C14" s="19"/>
       <c r="D14" s="17"/>
       <c r="E14" s="18" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F14" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="H14" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="I14" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="H14" s="18" t="s">
-        <v>143</v>
-      </c>
-      <c r="I14" s="18" t="s">
-        <v>114</v>
-      </c>
       <c r="J14" s="18" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="K14" s="18" t="s">
         <v>76</v>
@@ -8232,20 +8222,20 @@
       <c r="C15" s="20"/>
       <c r="D15" s="17"/>
       <c r="E15" s="21" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F15" s="22" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="G15" s="21"/>
       <c r="H15" s="18" t="s">
+        <v>145</v>
+      </c>
+      <c r="I15" s="18" t="s">
+        <v>146</v>
+      </c>
+      <c r="J15" s="18" t="s">
         <v>147</v>
-      </c>
-      <c r="I15" s="18" t="s">
-        <v>148</v>
-      </c>
-      <c r="J15" s="18" t="s">
-        <v>149</v>
       </c>
       <c r="K15" s="18" t="s">
         <v>54</v>
@@ -8287,20 +8277,20 @@
       <c r="C16" s="20"/>
       <c r="D16" s="17"/>
       <c r="E16" s="21" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F16" s="22" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="G16" s="21"/>
       <c r="H16" s="18" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="I16" s="18" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="J16" s="18" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="K16" s="18" t="s">
         <v>76</v>
@@ -8342,20 +8332,20 @@
       <c r="C17" s="20"/>
       <c r="D17" s="17"/>
       <c r="E17" s="21" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F17" s="22" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="G17" s="21"/>
       <c r="H17" s="18" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="I17" s="18" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="J17" s="18" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="K17" s="18" t="s">
         <v>76</v>
@@ -8397,20 +8387,20 @@
       <c r="C18" s="20"/>
       <c r="D18" s="17"/>
       <c r="E18" s="21" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F18" s="22" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="G18" s="21"/>
       <c r="H18" s="18" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I18" s="18" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="J18" s="18" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="K18" s="18" t="s">
         <v>76</v>
@@ -8452,20 +8442,20 @@
       <c r="C19" s="20"/>
       <c r="D19" s="17"/>
       <c r="E19" s="21" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F19" s="22" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="G19" s="21"/>
       <c r="H19" s="18" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="I19" s="18" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="J19" s="18" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="K19" s="18" t="s">
         <v>76</v>
@@ -8474,7 +8464,7 @@
       <c r="M19" s="18"/>
       <c r="N19" s="18"/>
       <c r="O19" s="18" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="P19" s="18"/>
       <c r="Q19" s="17"/>
@@ -8507,17 +8497,17 @@
       <c r="C20" s="20"/>
       <c r="D20" s="17"/>
       <c r="E20" s="21" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F20" s="22" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="G20" s="21"/>
       <c r="H20" s="18" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="I20" s="18" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="J20" s="18" t="s">
         <v>95</v>
@@ -8562,20 +8552,20 @@
       <c r="C21" s="20"/>
       <c r="D21" s="17"/>
       <c r="E21" s="21" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F21" s="22" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="G21" s="21"/>
       <c r="H21" s="18" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="I21" s="18" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="J21" s="18" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="K21" s="18" t="s">
         <v>76</v>
@@ -8616,20 +8606,20 @@
       <c r="C22" s="20"/>
       <c r="D22" s="17"/>
       <c r="E22" s="21" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F22" s="22" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="G22" s="21"/>
       <c r="H22" s="18" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I22" s="18" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="J22" s="18" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="K22" s="18" t="s">
         <v>76</v>
@@ -8638,7 +8628,7 @@
       <c r="M22" s="18"/>
       <c r="N22" s="18"/>
       <c r="O22" s="18" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="P22" s="18"/>
       <c r="Q22" s="17"/>
@@ -8671,20 +8661,20 @@
       <c r="C23" s="20"/>
       <c r="D23" s="17"/>
       <c r="E23" s="21" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F23" s="22" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="G23" s="21"/>
       <c r="H23" s="18" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="I23" s="18" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="J23" s="18" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="K23" s="18" t="s">
         <v>76</v>
@@ -8693,7 +8683,7 @@
       <c r="M23" s="18"/>
       <c r="N23" s="18"/>
       <c r="O23" s="18" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="P23" s="18"/>
       <c r="Q23" s="17"/>
@@ -8726,17 +8716,17 @@
       <c r="C24" s="20"/>
       <c r="D24" s="17"/>
       <c r="E24" s="21" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F24" s="22" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="G24" s="21"/>
       <c r="H24" s="18" t="s">
         <v>22</v>
       </c>
       <c r="I24" s="18" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="J24" s="18" t="s">
         <v>23</v>
@@ -8781,20 +8771,20 @@
       <c r="C25" s="20"/>
       <c r="D25" s="17"/>
       <c r="E25" s="21" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F25" s="22" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="G25" s="21"/>
       <c r="H25" s="18" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="I25" s="18" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="J25" s="18" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="K25" s="18" t="s">
         <v>76</v>
@@ -8836,20 +8826,20 @@
       <c r="C26" s="20"/>
       <c r="D26" s="17"/>
       <c r="E26" s="21" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F26" s="22" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="G26" s="21"/>
       <c r="H26" s="18" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="I26" s="18" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="J26" s="18" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="K26" s="18" t="s">
         <v>76</v>
@@ -8858,7 +8848,7 @@
       <c r="M26" s="18"/>
       <c r="N26" s="18"/>
       <c r="O26" s="18" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="P26" s="18"/>
       <c r="Q26" s="17"/>
@@ -8891,20 +8881,20 @@
       <c r="C27" s="20"/>
       <c r="D27" s="9"/>
       <c r="E27" s="21" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F27" s="22" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="G27" s="21"/>
       <c r="H27" s="18" t="s">
+        <v>145</v>
+      </c>
+      <c r="I27" s="18" t="s">
+        <v>171</v>
+      </c>
+      <c r="J27" s="18" t="s">
         <v>147</v>
-      </c>
-      <c r="I27" s="18" t="s">
-        <v>173</v>
-      </c>
-      <c r="J27" s="18" t="s">
-        <v>149</v>
       </c>
       <c r="K27" s="18" t="s">
         <v>54</v>
@@ -8946,20 +8936,20 @@
       <c r="C28" s="20"/>
       <c r="D28" s="9"/>
       <c r="E28" s="21" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F28" s="22" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="G28" s="21"/>
       <c r="H28" s="18" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I28" s="18" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J28" s="21" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="K28" s="21" t="s">
         <v>76</v>
@@ -9001,20 +8991,20 @@
       <c r="C29" s="20"/>
       <c r="D29" s="9"/>
       <c r="E29" s="21" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F29" s="22" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="G29" s="21"/>
       <c r="H29" s="18" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="I29" s="18" t="s">
+        <v>171</v>
+      </c>
+      <c r="J29" s="18" t="s">
         <v>173</v>
-      </c>
-      <c r="J29" s="18" t="s">
-        <v>175</v>
       </c>
       <c r="K29" s="18" t="s">
         <v>76</v>
@@ -9056,20 +9046,20 @@
       <c r="C30" s="20"/>
       <c r="D30" s="9"/>
       <c r="E30" s="21" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F30" s="22" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="G30" s="22"/>
       <c r="H30" s="17" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="I30" s="18" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J30" s="17" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="K30" s="17" t="s">
         <v>76</v>
@@ -9110,20 +9100,20 @@
       <c r="C31" s="20"/>
       <c r="D31" s="9"/>
       <c r="E31" s="21" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F31" s="22" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="G31" s="21"/>
       <c r="H31" s="18" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I31" s="18" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J31" s="18" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="K31" s="18" t="s">
         <v>76</v>
@@ -9132,7 +9122,7 @@
       <c r="M31" s="18"/>
       <c r="N31" s="18"/>
       <c r="O31" s="18" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="P31" s="18"/>
       <c r="Q31" s="17"/>
@@ -9165,20 +9155,20 @@
       <c r="C32" s="20"/>
       <c r="D32" s="9"/>
       <c r="E32" s="21" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F32" s="22" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="G32" s="21"/>
       <c r="H32" s="18" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="I32" s="18" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J32" s="18" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="K32" s="18" t="s">
         <v>76</v>
@@ -9187,7 +9177,7 @@
       <c r="M32" s="18"/>
       <c r="N32" s="18"/>
       <c r="O32" s="18" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="P32" s="18"/>
       <c r="Q32" s="17"/>
@@ -9220,20 +9210,20 @@
       <c r="C33" s="20"/>
       <c r="D33" s="9"/>
       <c r="E33" s="21" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F33" s="22" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="G33" s="21"/>
       <c r="H33" s="18" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="I33" s="18" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J33" s="18" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="K33" s="18" t="s">
         <v>76</v>
@@ -9274,20 +9264,20 @@
       <c r="C34" s="20"/>
       <c r="D34" s="9"/>
       <c r="E34" s="21" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F34" s="22" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="G34" s="21"/>
       <c r="H34" s="18" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="I34" s="18" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J34" s="18" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="K34" s="18" t="s">
         <v>76</v>
@@ -9296,7 +9286,7 @@
       <c r="M34" s="18"/>
       <c r="N34" s="18"/>
       <c r="O34" s="18" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="P34" s="18"/>
       <c r="Q34" s="17"/>
@@ -9326,19 +9316,19 @@
         <v>10</v>
       </c>
       <c r="E35" s="0" t="s">
+        <v>175</v>
+      </c>
+      <c r="F35" s="22" t="s">
+        <v>176</v>
+      </c>
+      <c r="H35" s="0" t="s">
         <v>177</v>
-      </c>
-      <c r="F35" s="22" t="s">
-        <v>178</v>
-      </c>
-      <c r="H35" s="0" t="s">
-        <v>179</v>
       </c>
       <c r="I35" s="0" t="s">
         <v>31</v>
       </c>
       <c r="J35" s="0" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="K35" s="0" t="s">
         <v>24</v>
@@ -9352,19 +9342,19 @@
         <v>20</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="H36" s="0" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="I36" s="0" t="s">
         <v>91</v>
       </c>
       <c r="J36" s="0" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="K36" s="0" t="s">
         <v>24</v>
@@ -9381,13 +9371,13 @@
         <v>20</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="H37" s="0" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="I37" s="0" t="s">
         <v>91</v>

</xml_diff>

<commit_message>
Support date ranges from templates
</commit_message>
<xml_diff>
--- a/editor-models/generated-models/src/main/resources/HeD_Templates.xlsx
+++ b/editor-models/generated-models/src/main/resources/HeD_Templates.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="2" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="643" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="1" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="643" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Demo Triggers" sheetId="1" state="visible" r:id="rId2"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="835" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="837" uniqueCount="221">
   <si>
     <t>Sequence ID</t>
   </si>
@@ -238,7 +238,10 @@
     <t>diagnosticEventTime</t>
   </si>
   <si>
-    <t>unit={days,years,months,hours,minutes,seconds}</t>
+    <t>0..1</t>
+  </si>
+  <si>
+    <t>value=365;unit={days,years,months,hours,minutes,seconds}</t>
   </si>
   <si>
     <t>Problem Effective within Date Range</t>
@@ -247,7 +250,7 @@
     <t>problemEffectiveTime</t>
   </si>
   <si>
-    <t>0..1</t>
+    <t>unit={days,years,months,hours,minutes,seconds}</t>
   </si>
   <si>
     <t>Status</t>
@@ -1013,7 +1016,7 @@
   <dimension ref="A1:R14"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="D1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="F5" activeCellId="1" pane="topLeft" sqref="39:40 F5"/>
+      <selection activeCell="F5" activeCellId="0" pane="topLeft" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1448,8 +1451,8 @@
   </sheetPr>
   <dimension ref="A1:R49"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="C1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="K15" activeCellId="1" pane="topLeft" sqref="39:40 K15"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="C1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="M18" activeCellId="0" pane="topLeft" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.1"/>
@@ -1629,10 +1632,10 @@
         <v>72</v>
       </c>
       <c r="K5" s="0" t="s">
-        <v>24</v>
+        <v>73</v>
       </c>
       <c r="M5" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="O5" s="0" t="s">
         <v>65</v>
@@ -1649,19 +1652,19 @@
         <v>67</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="I6" s="0" t="s">
         <v>69</v>
       </c>
       <c r="J6" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="K6" s="0" t="s">
-        <v>76</v>
+        <v>24</v>
       </c>
       <c r="M6" s="0" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="O6" s="0" t="s">
         <v>65</v>
@@ -1678,19 +1681,19 @@
         <v>67</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="I7" s="0" t="s">
         <v>69</v>
       </c>
       <c r="J7" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="K7" s="0" t="s">
         <v>24</v>
       </c>
       <c r="M7" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="O7" s="0" t="s">
         <v>34</v>
@@ -1704,7 +1707,7 @@
         <v>66</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H9" s="0" t="s">
         <v>68</v>
@@ -1733,7 +1736,7 @@
         <v>66</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H10" s="0" t="s">
         <v>71</v>
@@ -1745,10 +1748,10 @@
         <v>72</v>
       </c>
       <c r="K10" s="0" t="s">
-        <v>24</v>
+        <v>73</v>
       </c>
       <c r="M10" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="O10" s="0" t="s">
         <v>65</v>
@@ -1762,19 +1765,22 @@
         <v>66</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="I11" s="0" t="s">
         <v>69</v>
       </c>
       <c r="J11" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="K11" s="0" t="s">
-        <v>76</v>
+        <v>24</v>
+      </c>
+      <c r="M11" s="0" t="s">
+        <v>77</v>
       </c>
       <c r="O11" s="0" t="s">
         <v>65</v>
@@ -1788,22 +1794,22 @@
         <v>66</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="I12" s="0" t="s">
         <v>69</v>
       </c>
       <c r="J12" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="K12" s="0" t="s">
         <v>24</v>
       </c>
       <c r="M12" s="7" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="O12" s="0" t="s">
         <v>34</v>
@@ -1817,7 +1823,7 @@
         <v>66</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H14" s="0" t="s">
         <v>68</v>
@@ -1846,7 +1852,7 @@
         <v>66</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H15" s="0" t="s">
         <v>71</v>
@@ -1858,10 +1864,10 @@
         <v>72</v>
       </c>
       <c r="K15" s="0" t="s">
-        <v>24</v>
+        <v>73</v>
       </c>
       <c r="M15" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="O15" s="0" t="s">
         <v>65</v>
@@ -1875,19 +1881,22 @@
         <v>66</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="I16" s="0" t="s">
         <v>69</v>
       </c>
       <c r="J16" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="K16" s="0" t="s">
-        <v>76</v>
+        <v>24</v>
+      </c>
+      <c r="M16" s="0" t="s">
+        <v>77</v>
       </c>
       <c r="O16" s="0" t="s">
         <v>65</v>
@@ -1901,22 +1910,22 @@
         <v>66</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="I17" s="0" t="s">
         <v>69</v>
       </c>
       <c r="J17" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="K17" s="0" t="s">
         <v>24</v>
       </c>
       <c r="M17" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="O17" s="0" t="s">
         <v>34</v>
@@ -1930,10 +1939,10 @@
         <v>66</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H20" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="I20" s="0" t="s">
         <v>52</v>
@@ -1959,22 +1968,22 @@
         <v>66</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H21" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="I21" s="0" t="s">
         <v>52</v>
       </c>
       <c r="J21" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="K21" s="0" t="s">
         <v>24</v>
       </c>
       <c r="O21" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="23">
@@ -1982,25 +1991,25 @@
         <v>30</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H23" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="I23" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="J23" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="K23" s="0" t="s">
         <v>54</v>
       </c>
       <c r="M23" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="O23" s="0" t="s">
         <v>34</v>
@@ -2011,25 +2020,25 @@
         <v>30</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H24" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I24" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="J24" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="K24" s="0" t="s">
         <v>24</v>
       </c>
       <c r="O24" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="25">
@@ -2037,13 +2046,13 @@
         <v>40</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H25" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="I25" s="0" t="s">
         <v>31</v>
@@ -2066,19 +2075,19 @@
         <v>40</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H26" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="I26" s="0" t="s">
         <v>31</v>
       </c>
       <c r="J26" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="K26" s="0" t="s">
         <v>24</v>
@@ -2092,13 +2101,13 @@
         <v>50</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H28" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="I28" s="0" t="s">
         <v>52</v>
@@ -2121,25 +2130,25 @@
         <v>50</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H29" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="I29" s="0" t="s">
         <v>52</v>
       </c>
       <c r="J29" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="K29" s="0" t="s">
         <v>24</v>
       </c>
       <c r="M29" s="11" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="O29" s="0" t="s">
         <v>65</v>
@@ -2147,7 +2156,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="30">
       <c r="E30" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="31">
@@ -2155,13 +2164,13 @@
         <v>60</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H31" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="I31" s="0" t="s">
         <v>52</v>
@@ -2184,25 +2193,25 @@
         <v>60</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="F32" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="H32" s="0" t="s">
         <v>105</v>
-      </c>
-      <c r="H32" s="0" t="s">
-        <v>104</v>
       </c>
       <c r="I32" s="0" t="s">
         <v>52</v>
       </c>
       <c r="J32" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="K32" s="0" t="s">
         <v>24</v>
       </c>
       <c r="M32" s="11" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="O32" s="0" t="s">
         <v>65</v>
@@ -2219,10 +2228,10 @@
         <v>66</v>
       </c>
       <c r="F47" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="H47" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="I47" s="0" t="s">
         <v>69</v>
@@ -2240,7 +2249,7 @@
         <v>34</v>
       </c>
       <c r="P47" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="48">
@@ -2251,22 +2260,22 @@
         <v>66</v>
       </c>
       <c r="F48" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="H48" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="I48" s="0" t="s">
         <v>69</v>
       </c>
       <c r="J48" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="K48" s="0" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="O48" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="49">
@@ -2277,22 +2286,22 @@
         <v>66</v>
       </c>
       <c r="F49" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="H49" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="I49" s="0" t="s">
         <v>69</v>
       </c>
       <c r="J49" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="K49" s="0" t="s">
         <v>24</v>
       </c>
       <c r="M49" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="O49" s="0" t="s">
         <v>34</v>
@@ -2316,8 +2325,8 @@
   </sheetPr>
   <dimension ref="A1:AMF65536"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A17" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A40" activeCellId="0" pane="topLeft" sqref="39:40"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A5" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="A40" activeCellId="0" pane="topLeft" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.1"/>
@@ -2384,25 +2393,25 @@
       <c r="C2" s="17"/>
       <c r="D2" s="17"/>
       <c r="E2" s="18" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="H2" s="18" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="I2" s="18" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="J2" s="18" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="K2" s="18" t="s">
         <v>24</v>
       </c>
       <c r="O2" s="18" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="Q2" s="17"/>
       <c r="R2" s="17"/>
@@ -2845,22 +2854,22 @@
       <c r="C3" s="17"/>
       <c r="D3" s="17"/>
       <c r="E3" s="18" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F3" s="17" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="H3" s="18" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="I3" s="18" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="J3" s="18" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="K3" s="18" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="O3" s="18" t="s">
         <v>34</v>
@@ -3306,22 +3315,22 @@
       <c r="C4" s="17"/>
       <c r="D4" s="17"/>
       <c r="E4" s="18" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F4" s="17" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="H4" s="18" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="I4" s="18" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="J4" s="18" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="K4" s="18" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="O4" s="18" t="s">
         <v>34</v>
@@ -3767,22 +3776,22 @@
       <c r="C5" s="17"/>
       <c r="D5" s="17"/>
       <c r="E5" s="18" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F5" s="17" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="H5" s="18" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="I5" s="18" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="J5" s="18" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="K5" s="18" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="O5" s="18" t="s">
         <v>34</v>
@@ -4228,25 +4237,25 @@
       <c r="C6" s="17"/>
       <c r="D6" s="17"/>
       <c r="E6" s="18" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F6" s="17" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="H6" s="18" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="I6" s="18" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="J6" s="18" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="K6" s="18" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="O6" s="18" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="Q6" s="17"/>
       <c r="R6" s="17"/>
@@ -4689,25 +4698,25 @@
       <c r="C7" s="17"/>
       <c r="D7" s="17"/>
       <c r="E7" s="18" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F7" s="17" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="H7" s="18" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="I7" s="18" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="J7" s="18" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="K7" s="18" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="O7" s="18" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="Q7" s="17"/>
       <c r="R7" s="17"/>
@@ -5150,25 +5159,25 @@
       <c r="C8" s="17"/>
       <c r="D8" s="17"/>
       <c r="E8" s="18" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F8" s="17" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="H8" s="18" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="I8" s="18" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="J8" s="18" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="K8" s="18" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="O8" s="18" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="Q8" s="17"/>
       <c r="R8" s="17"/>
@@ -5611,25 +5620,25 @@
       <c r="C9" s="17"/>
       <c r="D9" s="17"/>
       <c r="E9" s="18" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F9" s="17" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="H9" s="18" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="I9" s="18" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="J9" s="18" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="K9" s="18" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="O9" s="18" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="Q9" s="17"/>
       <c r="R9" s="17"/>
@@ -6072,25 +6081,25 @@
       <c r="C10" s="17"/>
       <c r="D10" s="17"/>
       <c r="E10" s="18" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F10" s="17" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="H10" s="18" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="I10" s="18" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="J10" s="18" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="K10" s="18" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="O10" s="18" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="Q10" s="17"/>
       <c r="R10" s="17"/>
@@ -6533,25 +6542,25 @@
       <c r="C11" s="17"/>
       <c r="D11" s="17"/>
       <c r="E11" s="18" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F11" s="17" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="H11" s="18" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="I11" s="18" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="J11" s="18" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="K11" s="18" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="O11" s="18" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="Q11" s="17"/>
       <c r="R11" s="17"/>
@@ -6994,25 +7003,25 @@
       <c r="C12" s="17"/>
       <c r="D12" s="17"/>
       <c r="E12" s="18" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F12" s="17" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="H12" s="18" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="I12" s="18" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="J12" s="18" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="K12" s="18" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="O12" s="18" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="Q12" s="17"/>
       <c r="R12" s="17"/>
@@ -7455,25 +7464,25 @@
       <c r="C13" s="17"/>
       <c r="D13" s="17"/>
       <c r="E13" s="18" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F13" s="17" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="H13" s="18" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="I13" s="18" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="J13" s="18" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="K13" s="18" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="O13" s="18" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="Q13" s="17"/>
       <c r="R13" s="17"/>
@@ -7916,25 +7925,25 @@
       <c r="C14" s="19"/>
       <c r="D14" s="17"/>
       <c r="E14" s="18" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F14" s="17" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="H14" s="18" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="I14" s="18" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="J14" s="18" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="K14" s="18" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="O14" s="18" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="Q14" s="17"/>
       <c r="R14" s="17"/>
@@ -8377,20 +8386,20 @@
       <c r="C15" s="20"/>
       <c r="D15" s="17"/>
       <c r="E15" s="21" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F15" s="22" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="G15" s="21"/>
       <c r="H15" s="18" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="I15" s="18" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="J15" s="18" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="K15" s="18" t="s">
         <v>54</v>
@@ -8432,23 +8441,23 @@
       <c r="C16" s="20"/>
       <c r="D16" s="17"/>
       <c r="E16" s="21" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F16" s="22" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="G16" s="21"/>
       <c r="H16" s="18" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="I16" s="18" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="J16" s="18" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="K16" s="18" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="L16" s="18"/>
       <c r="M16" s="18"/>
@@ -8487,23 +8496,23 @@
       <c r="C17" s="20"/>
       <c r="D17" s="17"/>
       <c r="E17" s="21" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F17" s="22" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="G17" s="21"/>
       <c r="H17" s="18" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="I17" s="18" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="J17" s="18" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="K17" s="18" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="L17" s="18"/>
       <c r="M17" s="18"/>
@@ -8542,23 +8551,23 @@
       <c r="C18" s="20"/>
       <c r="D18" s="17"/>
       <c r="E18" s="21" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F18" s="22" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="G18" s="21"/>
       <c r="H18" s="18" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="I18" s="18" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="J18" s="18" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="K18" s="18" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="L18" s="18"/>
       <c r="M18" s="18"/>
@@ -8597,29 +8606,29 @@
       <c r="C19" s="20"/>
       <c r="D19" s="17"/>
       <c r="E19" s="21" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F19" s="22" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="G19" s="21"/>
       <c r="H19" s="18" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="I19" s="18" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="J19" s="18" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="K19" s="18" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="L19" s="18"/>
       <c r="M19" s="18"/>
       <c r="N19" s="18"/>
       <c r="O19" s="18" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="P19" s="18"/>
       <c r="Q19" s="17"/>
@@ -8652,29 +8661,29 @@
       <c r="C20" s="20"/>
       <c r="D20" s="17"/>
       <c r="E20" s="21" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F20" s="22" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="G20" s="21"/>
       <c r="H20" s="18" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="I20" s="18" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="J20" s="18" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="K20" s="18" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="L20" s="18"/>
       <c r="M20" s="18"/>
       <c r="N20" s="18"/>
       <c r="O20" s="18" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="P20" s="18"/>
       <c r="Q20" s="17"/>
@@ -8707,23 +8716,23 @@
       <c r="C21" s="20"/>
       <c r="D21" s="17"/>
       <c r="E21" s="21" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F21" s="22" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="G21" s="21"/>
       <c r="H21" s="18" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="I21" s="18" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="J21" s="18" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="K21" s="18" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="L21" s="18"/>
       <c r="M21" s="18"/>
@@ -8761,29 +8770,29 @@
       <c r="C22" s="20"/>
       <c r="D22" s="17"/>
       <c r="E22" s="21" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F22" s="22" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="G22" s="21"/>
       <c r="H22" s="18" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="I22" s="18" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="J22" s="18" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="K22" s="18" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="L22" s="18"/>
       <c r="M22" s="18"/>
       <c r="N22" s="18"/>
       <c r="O22" s="18" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="P22" s="18"/>
       <c r="Q22" s="17"/>
@@ -8816,29 +8825,29 @@
       <c r="C23" s="20"/>
       <c r="D23" s="17"/>
       <c r="E23" s="21" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F23" s="22" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="G23" s="21"/>
       <c r="H23" s="18" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="I23" s="18" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="J23" s="18" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="K23" s="18" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="L23" s="18"/>
       <c r="M23" s="18"/>
       <c r="N23" s="18"/>
       <c r="O23" s="18" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="P23" s="18"/>
       <c r="Q23" s="17"/>
@@ -8871,23 +8880,23 @@
       <c r="C24" s="20"/>
       <c r="D24" s="17"/>
       <c r="E24" s="21" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F24" s="22" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="G24" s="21"/>
       <c r="H24" s="18" t="s">
         <v>22</v>
       </c>
       <c r="I24" s="18" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="J24" s="18" t="s">
         <v>23</v>
       </c>
       <c r="K24" s="18" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="L24" s="18"/>
       <c r="M24" s="18"/>
@@ -8926,23 +8935,23 @@
       <c r="C25" s="20"/>
       <c r="D25" s="17"/>
       <c r="E25" s="21" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F25" s="22" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="G25" s="21"/>
       <c r="H25" s="18" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="I25" s="18" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="J25" s="18" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="K25" s="18" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="L25" s="18"/>
       <c r="M25" s="18"/>
@@ -8981,29 +8990,29 @@
       <c r="C26" s="20"/>
       <c r="D26" s="17"/>
       <c r="E26" s="21" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F26" s="22" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="G26" s="21"/>
       <c r="H26" s="18" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="I26" s="18" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="J26" s="18" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="K26" s="18" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="L26" s="18"/>
       <c r="M26" s="18"/>
       <c r="N26" s="18"/>
       <c r="O26" s="18" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="P26" s="18"/>
       <c r="Q26" s="17"/>
@@ -9036,20 +9045,20 @@
       <c r="C27" s="20"/>
       <c r="D27" s="9"/>
       <c r="E27" s="21" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F27" s="22" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="G27" s="21"/>
       <c r="H27" s="18" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="I27" s="18" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="J27" s="18" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="K27" s="18" t="s">
         <v>54</v>
@@ -9091,23 +9100,23 @@
       <c r="C28" s="20"/>
       <c r="D28" s="9"/>
       <c r="E28" s="21" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F28" s="22" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="G28" s="21"/>
       <c r="H28" s="18" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="I28" s="18" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="J28" s="21" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="K28" s="21" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="L28" s="21"/>
       <c r="M28" s="21"/>
@@ -9146,29 +9155,29 @@
       <c r="C29" s="20"/>
       <c r="D29" s="9"/>
       <c r="E29" s="21" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F29" s="22" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="G29" s="21"/>
       <c r="H29" s="18" t="s">
+        <v>174</v>
+      </c>
+      <c r="I29" s="18" t="s">
         <v>173</v>
       </c>
-      <c r="I29" s="18" t="s">
-        <v>172</v>
-      </c>
       <c r="J29" s="18" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="K29" s="18" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="L29" s="18"/>
       <c r="M29" s="18"/>
       <c r="N29" s="18"/>
       <c r="O29" s="18" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="P29" s="18"/>
       <c r="Q29" s="17"/>
@@ -9201,23 +9210,23 @@
       <c r="C30" s="20"/>
       <c r="D30" s="9"/>
       <c r="E30" s="21" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F30" s="22" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="G30" s="22"/>
       <c r="H30" s="17" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="I30" s="18" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="J30" s="17" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="K30" s="17" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="L30" s="17"/>
       <c r="M30" s="17"/>
@@ -9255,29 +9264,29 @@
       <c r="C31" s="20"/>
       <c r="D31" s="9"/>
       <c r="E31" s="21" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F31" s="22" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="G31" s="21"/>
       <c r="H31" s="18" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="I31" s="18" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="J31" s="18" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="K31" s="18" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="L31" s="18"/>
       <c r="M31" s="18"/>
       <c r="N31" s="18"/>
       <c r="O31" s="18" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="P31" s="18"/>
       <c r="Q31" s="17"/>
@@ -9310,29 +9319,29 @@
       <c r="C32" s="20"/>
       <c r="D32" s="9"/>
       <c r="E32" s="21" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F32" s="22" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="G32" s="21"/>
       <c r="H32" s="18" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="I32" s="18" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="J32" s="18" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="K32" s="18" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="L32" s="18"/>
       <c r="M32" s="18"/>
       <c r="N32" s="18"/>
       <c r="O32" s="18" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="P32" s="18"/>
       <c r="Q32" s="17"/>
@@ -9365,23 +9374,23 @@
       <c r="C33" s="20"/>
       <c r="D33" s="9"/>
       <c r="E33" s="21" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F33" s="22" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="G33" s="21"/>
       <c r="H33" s="18" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="I33" s="18" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="J33" s="18" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="K33" s="18" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="L33" s="18"/>
       <c r="M33" s="18"/>
@@ -9419,29 +9428,29 @@
       <c r="C34" s="20"/>
       <c r="D34" s="9"/>
       <c r="E34" s="21" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F34" s="22" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="G34" s="21"/>
       <c r="H34" s="18" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="I34" s="18" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="J34" s="18" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="K34" s="18" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="L34" s="18"/>
       <c r="M34" s="18"/>
       <c r="N34" s="18"/>
       <c r="O34" s="18" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="P34" s="18"/>
       <c r="Q34" s="17"/>
@@ -9471,19 +9480,19 @@
         <v>10</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="F35" s="22" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="H35" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="I35" s="0" t="s">
         <v>31</v>
       </c>
       <c r="J35" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="K35" s="0" t="s">
         <v>24</v>
@@ -9497,25 +9506,25 @@
         <v>20</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="H36" s="0" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="I36" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="J36" s="0" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="K36" s="0" t="s">
         <v>24</v>
       </c>
       <c r="M36" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="O36" s="0" t="s">
         <v>34</v>
@@ -9526,25 +9535,25 @@
         <v>20</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="H37" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="I37" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="J37" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="K37" s="0" t="s">
         <v>24</v>
       </c>
       <c r="O37" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="39" s="28">
@@ -9552,27 +9561,27 @@
         <v>30</v>
       </c>
       <c r="B39" s="25" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C39" s="25" t="n">
         <v>1</v>
       </c>
       <c r="D39" s="25"/>
       <c r="E39" s="18" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F39" s="26" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="G39" s="27"/>
       <c r="H39" s="28" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="I39" s="28" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="J39" s="28" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="K39" s="28" t="s">
         <v>24</v>
@@ -10132,30 +10141,30 @@
         <v>30</v>
       </c>
       <c r="B40" s="25" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C40" s="25" t="n">
         <v>1</v>
       </c>
       <c r="D40" s="25"/>
       <c r="E40" s="18" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F40" s="26" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="G40" s="27"/>
       <c r="H40" s="28" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="I40" s="28" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="J40" s="28" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="K40" s="28" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="O40" s="28" t="s">
         <v>34</v>
@@ -10712,33 +10721,33 @@
         <v>30</v>
       </c>
       <c r="B41" s="25" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C41" s="25" t="n">
         <v>1</v>
       </c>
       <c r="D41" s="25"/>
       <c r="E41" s="18" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F41" s="26" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="G41" s="27"/>
       <c r="H41" s="28" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="I41" s="28" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="J41" s="28" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="K41" s="28" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="O41" s="28" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="Q41" s="25"/>
       <c r="R41" s="25"/>
@@ -11292,30 +11301,30 @@
         <v>30</v>
       </c>
       <c r="B42" s="25" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C42" s="25" t="n">
         <v>1</v>
       </c>
       <c r="D42" s="25"/>
       <c r="E42" s="18" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F42" s="26" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="G42" s="27"/>
       <c r="H42" s="28" t="s">
         <v>22</v>
       </c>
       <c r="I42" s="28" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="J42" s="28" t="s">
         <v>23</v>
       </c>
       <c r="K42" s="28" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="L42" s="29"/>
       <c r="O42" s="28" t="s">
@@ -11915,33 +11924,33 @@
         <v>30</v>
       </c>
       <c r="B43" s="25" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C43" s="25" t="n">
         <v>1</v>
       </c>
       <c r="D43" s="25"/>
       <c r="E43" s="18" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F43" s="26" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="G43" s="27"/>
       <c r="H43" s="28" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="I43" s="28" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="J43" s="28" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="K43" s="28" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="O43" s="28" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="Q43" s="25"/>
       <c r="R43" s="25"/>
@@ -12495,30 +12504,30 @@
         <v>30</v>
       </c>
       <c r="B44" s="25" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C44" s="25" t="n">
         <v>1</v>
       </c>
       <c r="D44" s="25"/>
       <c r="E44" s="18" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F44" s="26" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="G44" s="27"/>
       <c r="H44" s="28" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="I44" s="28" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="J44" s="28" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="K44" s="28" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="O44" s="28" t="s">
         <v>34</v>
@@ -13075,30 +13084,30 @@
         <v>30</v>
       </c>
       <c r="B45" s="25" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C45" s="25" t="n">
         <v>1</v>
       </c>
       <c r="D45" s="25"/>
       <c r="E45" s="18" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F45" s="26" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="G45" s="27"/>
       <c r="H45" s="28" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="I45" s="28" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="J45" s="28" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="K45" s="28" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="O45" s="28" t="s">
         <v>34</v>
@@ -13655,24 +13664,24 @@
         <v>30</v>
       </c>
       <c r="B46" s="25" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C46" s="25" t="n">
         <v>1</v>
       </c>
       <c r="D46" s="25"/>
       <c r="E46" s="18" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F46" s="26" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="G46" s="27"/>
       <c r="H46" s="28" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="I46" s="28" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="J46" s="28" t="s">
         <v>53</v>
@@ -14235,30 +14244,30 @@
         <v>30</v>
       </c>
       <c r="B47" s="25" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C47" s="25" t="n">
         <v>1</v>
       </c>
       <c r="D47" s="25"/>
       <c r="E47" s="18" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F47" s="26" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="G47" s="27"/>
       <c r="H47" s="28" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="I47" s="28" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="J47" s="28" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="K47" s="28" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="O47" s="28" t="s">
         <v>34</v>
@@ -14815,33 +14824,33 @@
         <v>30</v>
       </c>
       <c r="B48" s="25" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C48" s="25" t="n">
         <v>1</v>
       </c>
       <c r="D48" s="25"/>
       <c r="E48" s="18" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F48" s="26" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="G48" s="27"/>
       <c r="H48" s="28" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="I48" s="28" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="J48" s="28" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="K48" s="28" t="s">
         <v>24</v>
       </c>
       <c r="O48" s="28" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="Q48" s="25"/>
       <c r="R48" s="25"/>
@@ -15395,30 +15404,30 @@
         <v>30</v>
       </c>
       <c r="B49" s="25" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C49" s="25" t="n">
         <v>1</v>
       </c>
       <c r="D49" s="25"/>
       <c r="E49" s="18" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F49" s="26" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="G49" s="27"/>
       <c r="H49" s="28" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="I49" s="28" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="J49" s="28" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="K49" s="28" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="O49" s="28" t="s">
         <v>34</v>
@@ -15975,30 +15984,30 @@
         <v>30</v>
       </c>
       <c r="B50" s="25" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C50" s="25" t="n">
         <v>1</v>
       </c>
       <c r="D50" s="25"/>
       <c r="E50" s="18" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F50" s="26" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="G50" s="27"/>
       <c r="H50" s="28" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="I50" s="28" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="J50" s="28" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="K50" s="28" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="O50" s="28" t="s">
         <v>34</v>
@@ -16555,30 +16564,30 @@
         <v>30</v>
       </c>
       <c r="B51" s="25" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C51" s="25" t="n">
         <v>1</v>
       </c>
       <c r="D51" s="25"/>
       <c r="E51" s="18" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F51" s="26" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="G51" s="27"/>
       <c r="H51" s="28" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="I51" s="28" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="J51" s="28" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="K51" s="28" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="O51" s="28" t="s">
         <v>34</v>
@@ -17135,30 +17144,30 @@
         <v>30</v>
       </c>
       <c r="B52" s="25" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C52" s="25" t="n">
         <v>1</v>
       </c>
       <c r="D52" s="25"/>
       <c r="E52" s="18" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F52" s="26" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="G52" s="27"/>
       <c r="H52" s="28" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="I52" s="28" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="J52" s="28" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="K52" s="28" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="O52" s="28" t="s">
         <v>34</v>
@@ -17715,27 +17724,27 @@
         <v>30</v>
       </c>
       <c r="B53" s="25" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C53" s="25" t="n">
         <v>1</v>
       </c>
       <c r="D53" s="25"/>
       <c r="E53" s="18" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F53" s="26" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="G53" s="27"/>
       <c r="H53" s="28" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="I53" s="28" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="J53" s="28" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="K53" s="28" t="s">
         <v>24</v>
@@ -18295,33 +18304,33 @@
         <v>30</v>
       </c>
       <c r="B54" s="25" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C54" s="25" t="n">
         <v>1</v>
       </c>
       <c r="D54" s="25"/>
       <c r="E54" s="18" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F54" s="26" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="G54" s="27"/>
       <c r="H54" s="28" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="I54" s="28" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="J54" s="28" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="K54" s="28" t="s">
         <v>24</v>
       </c>
       <c r="M54" s="28" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="O54" s="28" t="s">
         <v>34</v>
@@ -18878,30 +18887,30 @@
         <v>30</v>
       </c>
       <c r="B55" s="25" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C55" s="25" t="n">
         <v>1</v>
       </c>
       <c r="D55" s="25"/>
       <c r="E55" s="18" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F55" s="26" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="G55" s="27"/>
       <c r="H55" s="28" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="I55" s="28" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="J55" s="28" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="K55" s="28" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="O55" s="28" t="s">
         <v>34</v>
@@ -19458,30 +19467,30 @@
         <v>40</v>
       </c>
       <c r="B56" s="25" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C56" s="25" t="n">
         <v>1</v>
       </c>
       <c r="D56" s="25"/>
       <c r="E56" s="18" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F56" s="26" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="G56" s="27"/>
       <c r="H56" s="28" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="I56" s="28" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="J56" s="28" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="K56" s="28" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="O56" s="28" t="s">
         <v>34</v>
@@ -20038,30 +20047,30 @@
         <v>40</v>
       </c>
       <c r="B57" s="25" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C57" s="25" t="n">
         <v>1</v>
       </c>
       <c r="D57" s="25"/>
       <c r="E57" s="18" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F57" s="26" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="G57" s="27"/>
       <c r="H57" s="28" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="I57" s="28" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="J57" s="28" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="K57" s="28" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="O57" s="28" t="s">
         <v>34</v>
@@ -20618,30 +20627,30 @@
         <v>40</v>
       </c>
       <c r="B58" s="25" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C58" s="25" t="n">
         <v>1</v>
       </c>
       <c r="D58" s="25"/>
       <c r="E58" s="18" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F58" s="26" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="G58" s="27"/>
       <c r="H58" s="28" t="s">
         <v>22</v>
       </c>
       <c r="I58" s="28" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="J58" s="28" t="s">
         <v>23</v>
       </c>
       <c r="K58" s="28" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="L58" s="29"/>
       <c r="O58" s="28" t="s">
@@ -21241,33 +21250,33 @@
         <v>40</v>
       </c>
       <c r="B59" s="25" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C59" s="25" t="n">
         <v>1</v>
       </c>
       <c r="D59" s="25"/>
       <c r="E59" s="18" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F59" s="26" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="G59" s="27"/>
       <c r="H59" s="28" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="I59" s="28" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="J59" s="28" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="K59" s="28" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="O59" s="28" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="Q59" s="25"/>
       <c r="R59" s="25"/>
@@ -21821,30 +21830,30 @@
         <v>40</v>
       </c>
       <c r="B60" s="25" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C60" s="25" t="n">
         <v>1</v>
       </c>
       <c r="D60" s="25"/>
       <c r="E60" s="18" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F60" s="26" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="G60" s="27"/>
       <c r="H60" s="28" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="I60" s="28" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="J60" s="28" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="K60" s="28" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="O60" s="28" t="s">
         <v>34</v>
@@ -22401,30 +22410,30 @@
         <v>40</v>
       </c>
       <c r="B61" s="25" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C61" s="25" t="n">
         <v>1</v>
       </c>
       <c r="D61" s="25"/>
       <c r="E61" s="18" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F61" s="26" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="G61" s="27"/>
       <c r="H61" s="28" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="I61" s="28" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="J61" s="28" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="K61" s="28" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="O61" s="28" t="s">
         <v>34</v>
@@ -22981,24 +22990,24 @@
         <v>40</v>
       </c>
       <c r="B62" s="25" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C62" s="25" t="n">
         <v>1</v>
       </c>
       <c r="D62" s="25"/>
       <c r="E62" s="18" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F62" s="26" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="G62" s="27"/>
       <c r="H62" s="28" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="I62" s="28" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="J62" s="28" t="s">
         <v>53</v>
@@ -23561,33 +23570,33 @@
         <v>40</v>
       </c>
       <c r="B63" s="25" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C63" s="25" t="n">
         <v>1</v>
       </c>
       <c r="D63" s="25"/>
       <c r="E63" s="18" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F63" s="26" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="G63" s="27"/>
       <c r="H63" s="28" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="I63" s="28" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="J63" s="28" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="K63" s="28" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="O63" s="28" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="Q63" s="25"/>
       <c r="R63" s="25"/>
@@ -24141,30 +24150,30 @@
         <v>40</v>
       </c>
       <c r="B64" s="25" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C64" s="25" t="n">
         <v>1</v>
       </c>
       <c r="D64" s="25"/>
       <c r="E64" s="18" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F64" s="26" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="G64" s="27"/>
       <c r="H64" s="28" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="I64" s="28" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="J64" s="28" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="K64" s="28" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="O64" s="28" t="s">
         <v>34</v>
@@ -24721,30 +24730,30 @@
         <v>40</v>
       </c>
       <c r="B65" s="25" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C65" s="25" t="n">
         <v>1</v>
       </c>
       <c r="D65" s="25"/>
       <c r="E65" s="18" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F65" s="26" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="G65" s="27"/>
       <c r="H65" s="28" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="I65" s="28" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="J65" s="28" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="K65" s="28" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="O65" s="28" t="s">
         <v>34</v>
@@ -25301,33 +25310,33 @@
         <v>40</v>
       </c>
       <c r="B66" s="25" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C66" s="25" t="n">
         <v>1</v>
       </c>
       <c r="D66" s="25"/>
       <c r="E66" s="18" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F66" s="26" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="G66" s="27"/>
       <c r="H66" s="28" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="I66" s="28" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="J66" s="28" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="K66" s="28" t="s">
         <v>24</v>
       </c>
       <c r="M66" s="28" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="O66" s="28" t="s">
         <v>34</v>
@@ -25884,30 +25893,30 @@
         <v>40</v>
       </c>
       <c r="B67" s="25" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C67" s="25" t="n">
         <v>1</v>
       </c>
       <c r="D67" s="25"/>
       <c r="E67" s="18" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F67" s="26" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="G67" s="27"/>
       <c r="H67" s="28" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="I67" s="28" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="J67" s="28" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="K67" s="28" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="O67" s="28" t="s">
         <v>34</v>

</xml_diff>

<commit_message>
Ensure parameter attributes are sorted
</commit_message>
<xml_diff>
--- a/editor-models/generated-models/src/main/resources/HeD_Templates.xlsx
+++ b/editor-models/generated-models/src/main/resources/HeD_Templates.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="1" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="643" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="2" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="643" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Demo Triggers" sheetId="1" state="visible" r:id="rId2"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="837" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="837" uniqueCount="218">
   <si>
     <t>Sequence ID</t>
   </si>
@@ -220,7 +220,7 @@
     <t>Problem/Diagnosis, Condition</t>
   </si>
   <si>
-    <t>ProblemDiagnosis</t>
+    <t>ProblemOrDiagnosis</t>
   </si>
   <si>
     <t>Problem Type</t>
@@ -268,25 +268,22 @@
     <t>Date Range</t>
   </si>
   <si>
-    <t>valueSet=Problem Status;codeSystem=SHARP;code=resolved;displayValue=Problem Active</t>
+    <t>valueSet=Problem Status;codeSystem=SHARP;code=resolved;displayValue=Active Problem</t>
   </si>
   <si>
     <t>ResolvedProblemDiagnosis</t>
   </si>
   <si>
-    <t>valueSet=Problem Status;codeSystem=SHARP;code=resolved;displayValue=Problem Resolved</t>
+    <t>valueSet=Problem Status;codeSystem=SHARP;code=resolved;displayValue=Resolved Problem</t>
   </si>
   <si>
-    <t>StatusPostSurgery</t>
+    <t>PastSurgery</t>
   </si>
   <si>
     <t>Procedure</t>
   </si>
   <si>
     <t>procedureTime</t>
-  </si>
-  <si>
-    <t>IVL_TS</t>
   </si>
   <si>
     <t>Orders/Actions, Condition</t>
@@ -311,6 +308,9 @@
   </si>
   <si>
     <t>administrationTimeInterval</t>
+  </si>
+  <si>
+    <t>IVL_TS</t>
   </si>
   <si>
     <t>Observations/Results,Condition</t>
@@ -361,7 +361,7 @@
     <t>Message</t>
   </si>
   <si>
-    <t>CommunicationProposal/</t>
+    <t>CommunicationProposal</t>
   </si>
   <si>
     <t>message</t>
@@ -463,7 +463,7 @@
     <t>Substance Code</t>
   </si>
   <si>
-    <t>SubstanceAdministrationOrder/</t>
+    <t>SubstanceAdministrationOrder</t>
   </si>
   <si>
     <t>substance.substanceCode</t>
@@ -538,7 +538,7 @@
     <t>MedicationOrderReccomendation</t>
   </si>
   <si>
-    <t>SubstanceAdministrationProposal/</t>
+    <t>SubstanceAdministrationProposal</t>
   </si>
   <si>
     <t>Proposed Administration Time</t>
@@ -577,9 +577,6 @@
     <t>Approach Body Site</t>
   </si>
   <si>
-    <t>LaboratoryOrder/</t>
-  </si>
-  <si>
     <t>approachBodySite</t>
   </si>
   <si>
@@ -593,9 +590,6 @@
   </si>
   <si>
     <t>comment</t>
-  </si>
-  <si>
-    <t>Documentation</t>
   </si>
   <si>
     <t>Order Event Time</t>
@@ -674,9 +668,6 @@
   </si>
   <si>
     <t>ProcedureOrder</t>
-  </si>
-  <si>
-    <t>ProcedureOrder/</t>
   </si>
   <si>
     <t>0..*</t>
@@ -1451,8 +1442,8 @@
   </sheetPr>
   <dimension ref="A1:R49"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="C1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="M18" activeCellId="0" pane="topLeft" sqref="M18"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="C1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="F22" activeCellId="0" pane="topLeft" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.1"/>
@@ -1983,7 +1974,7 @@
         <v>24</v>
       </c>
       <c r="O21" s="0" t="s">
-        <v>89</v>
+        <v>65</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="23">
@@ -1991,25 +1982,25 @@
         <v>30</v>
       </c>
       <c r="E23" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="F23" s="0" t="s">
         <v>90</v>
       </c>
-      <c r="F23" s="0" t="s">
+      <c r="H23" s="0" t="s">
         <v>91</v>
       </c>
-      <c r="H23" s="0" t="s">
+      <c r="I23" s="0" t="s">
         <v>92</v>
       </c>
-      <c r="I23" s="0" t="s">
+      <c r="J23" s="0" t="s">
         <v>93</v>
-      </c>
-      <c r="J23" s="0" t="s">
-        <v>94</v>
       </c>
       <c r="K23" s="0" t="s">
         <v>54</v>
       </c>
       <c r="M23" s="0" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="O23" s="0" t="s">
         <v>34</v>
@@ -2020,25 +2011,25 @@
         <v>30</v>
       </c>
       <c r="E24" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="F24" s="0" t="s">
         <v>90</v>
       </c>
-      <c r="F24" s="0" t="s">
-        <v>91</v>
-      </c>
       <c r="H24" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="I24" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="J24" s="0" t="s">
         <v>96</v>
-      </c>
-      <c r="I24" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="J24" s="0" t="s">
-        <v>97</v>
       </c>
       <c r="K24" s="0" t="s">
         <v>24</v>
       </c>
       <c r="O24" s="0" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="25">
@@ -2275,7 +2266,7 @@
         <v>73</v>
       </c>
       <c r="O48" s="0" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="49">
@@ -2325,8 +2316,8 @@
   </sheetPr>
   <dimension ref="A1:AMF65536"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A5" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A40" activeCellId="0" pane="topLeft" sqref="A40"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="G1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="Q42" activeCellId="0" pane="topLeft" sqref="Q42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.1"/>
@@ -7943,7 +7934,7 @@
         <v>73</v>
       </c>
       <c r="O14" s="18" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="Q14" s="17"/>
       <c r="R14" s="17"/>
@@ -8674,7 +8665,7 @@
         <v>148</v>
       </c>
       <c r="J20" s="18" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K20" s="18" t="s">
         <v>73</v>
@@ -8683,7 +8674,7 @@
       <c r="M20" s="18"/>
       <c r="N20" s="18"/>
       <c r="O20" s="18" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="P20" s="18"/>
       <c r="Q20" s="17"/>
@@ -9177,7 +9168,7 @@
       <c r="M29" s="18"/>
       <c r="N29" s="18"/>
       <c r="O29" s="18" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="P29" s="18"/>
       <c r="Q29" s="17"/>
@@ -9515,7 +9506,7 @@
         <v>181</v>
       </c>
       <c r="I36" s="0" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J36" s="0" t="s">
         <v>182</v>
@@ -9524,7 +9515,7 @@
         <v>24</v>
       </c>
       <c r="M36" s="0" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="O36" s="0" t="s">
         <v>34</v>
@@ -9544,16 +9535,16 @@
         <v>159</v>
       </c>
       <c r="I37" s="0" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J37" s="0" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K37" s="0" t="s">
         <v>24</v>
       </c>
       <c r="O37" s="0" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="39" s="28">
@@ -9578,10 +9569,10 @@
         <v>185</v>
       </c>
       <c r="I39" s="28" t="s">
+        <v>184</v>
+      </c>
+      <c r="J39" s="28" t="s">
         <v>186</v>
-      </c>
-      <c r="J39" s="28" t="s">
-        <v>187</v>
       </c>
       <c r="K39" s="28" t="s">
         <v>24</v>
@@ -10155,13 +10146,13 @@
       </c>
       <c r="G40" s="27"/>
       <c r="H40" s="28" t="s">
+        <v>187</v>
+      </c>
+      <c r="I40" s="28" t="s">
+        <v>184</v>
+      </c>
+      <c r="J40" s="28" t="s">
         <v>188</v>
-      </c>
-      <c r="I40" s="28" t="s">
-        <v>186</v>
-      </c>
-      <c r="J40" s="28" t="s">
-        <v>189</v>
       </c>
       <c r="K40" s="28" t="s">
         <v>73</v>
@@ -10735,19 +10726,19 @@
       </c>
       <c r="G41" s="27"/>
       <c r="H41" s="28" t="s">
+        <v>189</v>
+      </c>
+      <c r="I41" s="28" t="s">
+        <v>184</v>
+      </c>
+      <c r="J41" s="28" t="s">
         <v>190</v>
-      </c>
-      <c r="I41" s="28" t="s">
-        <v>186</v>
-      </c>
-      <c r="J41" s="28" t="s">
-        <v>191</v>
       </c>
       <c r="K41" s="28" t="s">
         <v>73</v>
       </c>
       <c r="O41" s="28" t="s">
-        <v>192</v>
+        <v>116</v>
       </c>
       <c r="Q41" s="25"/>
       <c r="R41" s="25"/>
@@ -11318,7 +11309,7 @@
         <v>22</v>
       </c>
       <c r="I42" s="28" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="J42" s="28" t="s">
         <v>23</v>
@@ -11938,19 +11929,19 @@
       </c>
       <c r="G43" s="27"/>
       <c r="H43" s="28" t="s">
+        <v>191</v>
+      </c>
+      <c r="I43" s="28" t="s">
+        <v>184</v>
+      </c>
+      <c r="J43" s="28" t="s">
+        <v>192</v>
+      </c>
+      <c r="K43" s="28" t="s">
         <v>193</v>
       </c>
-      <c r="I43" s="28" t="s">
-        <v>186</v>
-      </c>
-      <c r="J43" s="28" t="s">
-        <v>194</v>
-      </c>
-      <c r="K43" s="28" t="s">
-        <v>195</v>
-      </c>
       <c r="O43" s="28" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="Q43" s="25"/>
       <c r="R43" s="25"/>
@@ -12518,16 +12509,16 @@
       </c>
       <c r="G44" s="27"/>
       <c r="H44" s="28" t="s">
+        <v>194</v>
+      </c>
+      <c r="I44" s="28" t="s">
+        <v>184</v>
+      </c>
+      <c r="J44" s="28" t="s">
+        <v>195</v>
+      </c>
+      <c r="K44" s="28" t="s">
         <v>196</v>
-      </c>
-      <c r="I44" s="28" t="s">
-        <v>186</v>
-      </c>
-      <c r="J44" s="28" t="s">
-        <v>197</v>
-      </c>
-      <c r="K44" s="28" t="s">
-        <v>198</v>
       </c>
       <c r="O44" s="28" t="s">
         <v>34</v>
@@ -13098,16 +13089,16 @@
       </c>
       <c r="G45" s="27"/>
       <c r="H45" s="28" t="s">
+        <v>197</v>
+      </c>
+      <c r="I45" s="28" t="s">
+        <v>184</v>
+      </c>
+      <c r="J45" s="28" t="s">
+        <v>198</v>
+      </c>
+      <c r="K45" s="28" t="s">
         <v>199</v>
-      </c>
-      <c r="I45" s="28" t="s">
-        <v>186</v>
-      </c>
-      <c r="J45" s="28" t="s">
-        <v>200</v>
-      </c>
-      <c r="K45" s="28" t="s">
-        <v>201</v>
       </c>
       <c r="O45" s="28" t="s">
         <v>34</v>
@@ -13678,10 +13669,10 @@
       </c>
       <c r="G46" s="27"/>
       <c r="H46" s="28" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="I46" s="28" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="J46" s="28" t="s">
         <v>53</v>
@@ -14258,13 +14249,13 @@
       </c>
       <c r="G47" s="27"/>
       <c r="H47" s="28" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="I47" s="28" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="J47" s="28" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="K47" s="28" t="s">
         <v>73</v>
@@ -14838,10 +14829,10 @@
       </c>
       <c r="G48" s="27"/>
       <c r="H48" s="28" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="I48" s="28" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="J48" s="28" t="s">
         <v>88</v>
@@ -14850,7 +14841,7 @@
         <v>24</v>
       </c>
       <c r="O48" s="28" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="Q48" s="25"/>
       <c r="R48" s="25"/>
@@ -15418,10 +15409,10 @@
       </c>
       <c r="G49" s="27"/>
       <c r="H49" s="28" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="I49" s="28" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="J49" s="28" t="s">
         <v>122</v>
@@ -15998,13 +15989,13 @@
       </c>
       <c r="G50" s="27"/>
       <c r="H50" s="28" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="I50" s="28" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="J50" s="28" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="K50" s="28" t="s">
         <v>73</v>
@@ -16578,16 +16569,16 @@
       </c>
       <c r="G51" s="27"/>
       <c r="H51" s="28" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="I51" s="28" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="J51" s="28" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="K51" s="28" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="O51" s="28" t="s">
         <v>34</v>
@@ -17158,16 +17149,16 @@
       </c>
       <c r="G52" s="27"/>
       <c r="H52" s="28" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="I52" s="28" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="J52" s="28" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="K52" s="28" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="O52" s="28" t="s">
         <v>34</v>
@@ -17738,13 +17729,13 @@
       </c>
       <c r="G53" s="27"/>
       <c r="H53" s="28" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="I53" s="28" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="J53" s="28" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="K53" s="28" t="s">
         <v>24</v>
@@ -18318,19 +18309,19 @@
       </c>
       <c r="G54" s="27"/>
       <c r="H54" s="28" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="I54" s="28" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="J54" s="28" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="K54" s="28" t="s">
         <v>24</v>
       </c>
       <c r="M54" s="28" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="O54" s="28" t="s">
         <v>34</v>
@@ -18904,7 +18895,7 @@
         <v>117</v>
       </c>
       <c r="I55" s="28" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="J55" s="28" t="s">
         <v>118</v>
@@ -19477,17 +19468,17 @@
         <v>145</v>
       </c>
       <c r="F56" s="26" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="G56" s="27"/>
       <c r="H56" s="28" t="s">
         <v>185</v>
       </c>
       <c r="I56" s="28" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="J56" s="28" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K56" s="28" t="s">
         <v>73</v>
@@ -20057,17 +20048,17 @@
         <v>145</v>
       </c>
       <c r="F57" s="26" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="G57" s="27"/>
       <c r="H57" s="28" t="s">
+        <v>189</v>
+      </c>
+      <c r="I57" s="28" t="s">
+        <v>216</v>
+      </c>
+      <c r="J57" s="28" t="s">
         <v>190</v>
-      </c>
-      <c r="I57" s="28" t="s">
-        <v>219</v>
-      </c>
-      <c r="J57" s="28" t="s">
-        <v>191</v>
       </c>
       <c r="K57" s="28" t="s">
         <v>73</v>
@@ -20637,14 +20628,14 @@
         <v>145</v>
       </c>
       <c r="F58" s="26" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="G58" s="27"/>
       <c r="H58" s="28" t="s">
         <v>22</v>
       </c>
       <c r="I58" s="28" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="J58" s="28" t="s">
         <v>23</v>
@@ -21260,23 +21251,23 @@
         <v>145</v>
       </c>
       <c r="F59" s="26" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="G59" s="27"/>
       <c r="H59" s="28" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="I59" s="28" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="J59" s="28" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="K59" s="28" t="s">
         <v>73</v>
       </c>
       <c r="O59" s="28" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="Q59" s="25"/>
       <c r="R59" s="25"/>
@@ -21840,17 +21831,17 @@
         <v>145</v>
       </c>
       <c r="F60" s="26" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="G60" s="27"/>
       <c r="H60" s="28" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="I60" s="28" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="J60" s="28" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="K60" s="28" t="s">
         <v>73</v>
@@ -22420,20 +22411,20 @@
         <v>145</v>
       </c>
       <c r="F61" s="26" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="G61" s="27"/>
       <c r="H61" s="28" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="I61" s="28" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="J61" s="28" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="K61" s="28" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="O61" s="28" t="s">
         <v>34</v>
@@ -23000,14 +22991,14 @@
         <v>145</v>
       </c>
       <c r="F62" s="26" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="G62" s="27"/>
       <c r="H62" s="28" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="I62" s="28" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="J62" s="28" t="s">
         <v>53</v>
@@ -23580,14 +23571,14 @@
         <v>145</v>
       </c>
       <c r="F63" s="26" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="G63" s="27"/>
       <c r="H63" s="28" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="I63" s="28" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="J63" s="28" t="s">
         <v>88</v>
@@ -23596,7 +23587,7 @@
         <v>73</v>
       </c>
       <c r="O63" s="28" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="Q63" s="25"/>
       <c r="R63" s="25"/>
@@ -24160,14 +24151,14 @@
         <v>145</v>
       </c>
       <c r="F64" s="26" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="G64" s="27"/>
       <c r="H64" s="28" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="I64" s="28" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="J64" s="28" t="s">
         <v>122</v>
@@ -24740,17 +24731,17 @@
         <v>145</v>
       </c>
       <c r="F65" s="26" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="G65" s="27"/>
       <c r="H65" s="28" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="I65" s="28" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="J65" s="28" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="K65" s="28" t="s">
         <v>73</v>
@@ -25320,23 +25311,23 @@
         <v>145</v>
       </c>
       <c r="F66" s="26" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="G66" s="27"/>
       <c r="H66" s="28" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="I66" s="28" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="J66" s="28" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="K66" s="28" t="s">
         <v>24</v>
       </c>
       <c r="M66" s="28" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="O66" s="28" t="s">
         <v>34</v>
@@ -25903,14 +25894,14 @@
         <v>145</v>
       </c>
       <c r="F67" s="26" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="G67" s="27"/>
       <c r="H67" s="28" t="s">
         <v>117</v>
       </c>
       <c r="I67" s="28" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="J67" s="28" t="s">
         <v>118</v>

</xml_diff>

<commit_message>
Enable template binding example
</commit_message>
<xml_diff>
--- a/editor-models/generated-models/src/main/resources/HeD_Templates.xlsx
+++ b/editor-models/generated-models/src/main/resources/HeD_Templates.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="2" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="643" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="1" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="643" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Demo Triggers" sheetId="1" state="visible" r:id="rId2"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="837" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="840" uniqueCount="218">
   <si>
     <t>Sequence ID</t>
   </si>
@@ -232,6 +232,9 @@
     <t>problemCode</t>
   </si>
   <si>
+    <t>SNOMED:127337006</t>
+  </si>
+  <si>
     <t>Problem Diagnosed within Date Range</t>
   </si>
   <si>
@@ -344,9 +347,6 @@
   </si>
   <si>
     <t>Cardiac Problem Type</t>
-  </si>
-  <si>
-    <t>SNOMED:127337006</t>
   </si>
   <si>
     <t>codeSystem=TBD;code=active</t>
@@ -1442,8 +1442,8 @@
   </sheetPr>
   <dimension ref="A1:R49"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="C1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="F22" activeCellId="0" pane="topLeft" sqref="F22"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="F1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="P24" activeCellId="0" pane="topLeft" sqref="P24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.1"/>
@@ -1602,6 +1602,9 @@
       <c r="O4" s="0" t="s">
         <v>34</v>
       </c>
+      <c r="P4" s="0" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="5">
       <c r="A5" s="0" t="n">
@@ -1614,19 +1617,19 @@
         <v>67</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="I5" s="0" t="s">
         <v>69</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="K5" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="M5" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="O5" s="0" t="s">
         <v>65</v>
@@ -1643,19 +1646,19 @@
         <v>67</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I6" s="0" t="s">
         <v>69</v>
       </c>
       <c r="J6" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="K6" s="0" t="s">
         <v>24</v>
       </c>
       <c r="M6" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="O6" s="0" t="s">
         <v>65</v>
@@ -1672,19 +1675,19 @@
         <v>67</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="I7" s="0" t="s">
         <v>69</v>
       </c>
       <c r="J7" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="K7" s="0" t="s">
         <v>24</v>
       </c>
       <c r="M7" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="O7" s="0" t="s">
         <v>34</v>
@@ -1698,7 +1701,7 @@
         <v>66</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H9" s="0" t="s">
         <v>68</v>
@@ -1717,6 +1720,9 @@
       </c>
       <c r="O9" s="0" t="s">
         <v>34</v>
+      </c>
+      <c r="P9" s="0" t="s">
+        <v>71</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="10">
@@ -1727,22 +1733,22 @@
         <v>66</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="I10" s="0" t="s">
         <v>69</v>
       </c>
       <c r="J10" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="K10" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="M10" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="O10" s="0" t="s">
         <v>65</v>
@@ -1756,22 +1762,22 @@
         <v>66</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="I11" s="0" t="s">
         <v>69</v>
       </c>
       <c r="J11" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="K11" s="0" t="s">
         <v>24</v>
       </c>
       <c r="M11" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="O11" s="0" t="s">
         <v>65</v>
@@ -1785,22 +1791,22 @@
         <v>66</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="I12" s="0" t="s">
         <v>69</v>
       </c>
       <c r="J12" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="K12" s="0" t="s">
         <v>24</v>
       </c>
       <c r="M12" s="7" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="O12" s="0" t="s">
         <v>34</v>
@@ -1814,7 +1820,7 @@
         <v>66</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H14" s="0" t="s">
         <v>68</v>
@@ -1833,6 +1839,9 @@
       </c>
       <c r="O14" s="0" t="s">
         <v>34</v>
+      </c>
+      <c r="P14" s="0" t="s">
+        <v>71</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="15">
@@ -1843,22 +1852,22 @@
         <v>66</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="I15" s="0" t="s">
         <v>69</v>
       </c>
       <c r="J15" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="K15" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="M15" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="O15" s="0" t="s">
         <v>65</v>
@@ -1872,22 +1881,22 @@
         <v>66</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="I16" s="0" t="s">
         <v>69</v>
       </c>
       <c r="J16" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="K16" s="0" t="s">
         <v>24</v>
       </c>
       <c r="M16" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="O16" s="0" t="s">
         <v>65</v>
@@ -1901,22 +1910,22 @@
         <v>66</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="I17" s="0" t="s">
         <v>69</v>
       </c>
       <c r="J17" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="K17" s="0" t="s">
         <v>24</v>
       </c>
       <c r="M17" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="O17" s="0" t="s">
         <v>34</v>
@@ -1930,10 +1939,10 @@
         <v>66</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H20" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="I20" s="0" t="s">
         <v>52</v>
@@ -1959,16 +1968,16 @@
         <v>66</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H21" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="I21" s="0" t="s">
         <v>52</v>
       </c>
       <c r="J21" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K21" s="0" t="s">
         <v>24</v>
@@ -1982,25 +1991,25 @@
         <v>30</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H23" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="I23" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="J23" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="K23" s="0" t="s">
         <v>54</v>
       </c>
       <c r="M23" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="O23" s="0" t="s">
         <v>34</v>
@@ -2011,25 +2020,25 @@
         <v>30</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H24" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I24" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="J24" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="K24" s="0" t="s">
         <v>24</v>
       </c>
       <c r="O24" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="25">
@@ -2037,13 +2046,13 @@
         <v>40</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H25" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="I25" s="0" t="s">
         <v>31</v>
@@ -2066,19 +2075,19 @@
         <v>40</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H26" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="I26" s="0" t="s">
         <v>31</v>
       </c>
       <c r="J26" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="K26" s="0" t="s">
         <v>24</v>
@@ -2092,13 +2101,13 @@
         <v>50</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H28" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="I28" s="0" t="s">
         <v>52</v>
@@ -2121,25 +2130,25 @@
         <v>50</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H29" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="I29" s="0" t="s">
         <v>52</v>
       </c>
       <c r="J29" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K29" s="0" t="s">
         <v>24</v>
       </c>
       <c r="M29" s="11" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="O29" s="0" t="s">
         <v>65</v>
@@ -2147,7 +2156,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="30">
       <c r="E30" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="31">
@@ -2155,13 +2164,13 @@
         <v>60</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="H31" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="I31" s="0" t="s">
         <v>52</v>
@@ -2184,25 +2193,25 @@
         <v>60</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="F32" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="H32" s="0" t="s">
         <v>106</v>
-      </c>
-      <c r="H32" s="0" t="s">
-        <v>105</v>
       </c>
       <c r="I32" s="0" t="s">
         <v>52</v>
       </c>
       <c r="J32" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K32" s="0" t="s">
         <v>24</v>
       </c>
       <c r="M32" s="11" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="O32" s="0" t="s">
         <v>65</v>
@@ -2219,10 +2228,10 @@
         <v>66</v>
       </c>
       <c r="F47" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H47" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="I47" s="0" t="s">
         <v>69</v>
@@ -2240,7 +2249,7 @@
         <v>34</v>
       </c>
       <c r="P47" s="0" t="s">
-        <v>109</v>
+        <v>71</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="48">
@@ -2251,22 +2260,22 @@
         <v>66</v>
       </c>
       <c r="F48" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H48" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="I48" s="0" t="s">
         <v>69</v>
       </c>
       <c r="J48" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="K48" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="O48" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="49">
@@ -2277,16 +2286,16 @@
         <v>66</v>
       </c>
       <c r="F49" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H49" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="I49" s="0" t="s">
         <v>69</v>
       </c>
       <c r="J49" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="K49" s="0" t="s">
         <v>24</v>
@@ -2316,7 +2325,7 @@
   </sheetPr>
   <dimension ref="A1:AMF65536"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="G1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="G1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="Q42" activeCellId="0" pane="topLeft" sqref="Q42"/>
     </sheetView>
   </sheetViews>
@@ -2860,7 +2869,7 @@
         <v>118</v>
       </c>
       <c r="K3" s="18" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="O3" s="18" t="s">
         <v>34</v>
@@ -3321,7 +3330,7 @@
         <v>120</v>
       </c>
       <c r="K4" s="18" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="O4" s="18" t="s">
         <v>34</v>
@@ -3782,7 +3791,7 @@
         <v>122</v>
       </c>
       <c r="K5" s="18" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="O5" s="18" t="s">
         <v>34</v>
@@ -4243,7 +4252,7 @@
         <v>124</v>
       </c>
       <c r="K6" s="18" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="O6" s="18" t="s">
         <v>125</v>
@@ -4704,7 +4713,7 @@
         <v>127</v>
       </c>
       <c r="K7" s="18" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="O7" s="18" t="s">
         <v>128</v>
@@ -5165,7 +5174,7 @@
         <v>130</v>
       </c>
       <c r="K8" s="18" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="O8" s="18" t="s">
         <v>131</v>
@@ -5626,7 +5635,7 @@
         <v>133</v>
       </c>
       <c r="K9" s="18" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="O9" s="18" t="s">
         <v>134</v>
@@ -6087,7 +6096,7 @@
         <v>136</v>
       </c>
       <c r="K10" s="18" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="O10" s="18" t="s">
         <v>125</v>
@@ -6548,7 +6557,7 @@
         <v>138</v>
       </c>
       <c r="K11" s="18" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="O11" s="18" t="s">
         <v>128</v>
@@ -7009,7 +7018,7 @@
         <v>140</v>
       </c>
       <c r="K12" s="18" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="O12" s="18" t="s">
         <v>131</v>
@@ -7470,7 +7479,7 @@
         <v>142</v>
       </c>
       <c r="K13" s="18" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="O13" s="18" t="s">
         <v>134</v>
@@ -7931,10 +7940,10 @@
         <v>144</v>
       </c>
       <c r="K14" s="18" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="O14" s="18" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="Q14" s="17"/>
       <c r="R14" s="17"/>
@@ -8448,7 +8457,7 @@
         <v>151</v>
       </c>
       <c r="K16" s="18" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="L16" s="18"/>
       <c r="M16" s="18"/>
@@ -8503,7 +8512,7 @@
         <v>153</v>
       </c>
       <c r="K17" s="18" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="L17" s="18"/>
       <c r="M17" s="18"/>
@@ -8558,7 +8567,7 @@
         <v>155</v>
       </c>
       <c r="K18" s="18" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="L18" s="18"/>
       <c r="M18" s="18"/>
@@ -8613,7 +8622,7 @@
         <v>157</v>
       </c>
       <c r="K19" s="18" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="L19" s="18"/>
       <c r="M19" s="18"/>
@@ -8665,16 +8674,16 @@
         <v>148</v>
       </c>
       <c r="J20" s="18" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="K20" s="18" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="L20" s="18"/>
       <c r="M20" s="18"/>
       <c r="N20" s="18"/>
       <c r="O20" s="18" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="P20" s="18"/>
       <c r="Q20" s="17"/>
@@ -8723,7 +8732,7 @@
         <v>161</v>
       </c>
       <c r="K21" s="18" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="L21" s="18"/>
       <c r="M21" s="18"/>
@@ -8777,7 +8786,7 @@
         <v>163</v>
       </c>
       <c r="K22" s="18" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="L22" s="18"/>
       <c r="M22" s="18"/>
@@ -8832,7 +8841,7 @@
         <v>166</v>
       </c>
       <c r="K23" s="18" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="L23" s="18"/>
       <c r="M23" s="18"/>
@@ -8887,7 +8896,7 @@
         <v>23</v>
       </c>
       <c r="K24" s="18" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="L24" s="18"/>
       <c r="M24" s="18"/>
@@ -8942,7 +8951,7 @@
         <v>168</v>
       </c>
       <c r="K25" s="18" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="L25" s="18"/>
       <c r="M25" s="18"/>
@@ -8997,7 +9006,7 @@
         <v>170</v>
       </c>
       <c r="K26" s="18" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="L26" s="18"/>
       <c r="M26" s="18"/>
@@ -9107,7 +9116,7 @@
         <v>155</v>
       </c>
       <c r="K28" s="21" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="L28" s="21"/>
       <c r="M28" s="21"/>
@@ -9162,13 +9171,13 @@
         <v>175</v>
       </c>
       <c r="K29" s="18" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="L29" s="18"/>
       <c r="M29" s="18"/>
       <c r="N29" s="18"/>
       <c r="O29" s="18" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="P29" s="18"/>
       <c r="Q29" s="17"/>
@@ -9217,7 +9226,7 @@
         <v>161</v>
       </c>
       <c r="K30" s="17" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="L30" s="17"/>
       <c r="M30" s="17"/>
@@ -9271,7 +9280,7 @@
         <v>163</v>
       </c>
       <c r="K31" s="18" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="L31" s="18"/>
       <c r="M31" s="18"/>
@@ -9326,7 +9335,7 @@
         <v>166</v>
       </c>
       <c r="K32" s="18" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="L32" s="18"/>
       <c r="M32" s="18"/>
@@ -9381,7 +9390,7 @@
         <v>168</v>
       </c>
       <c r="K33" s="18" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="L33" s="18"/>
       <c r="M33" s="18"/>
@@ -9435,7 +9444,7 @@
         <v>170</v>
       </c>
       <c r="K34" s="18" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="L34" s="18"/>
       <c r="M34" s="18"/>
@@ -9483,7 +9492,7 @@
         <v>31</v>
       </c>
       <c r="J35" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="K35" s="0" t="s">
         <v>24</v>
@@ -9506,7 +9515,7 @@
         <v>181</v>
       </c>
       <c r="I36" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="J36" s="0" t="s">
         <v>182</v>
@@ -9515,7 +9524,7 @@
         <v>24</v>
       </c>
       <c r="M36" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="O36" s="0" t="s">
         <v>34</v>
@@ -9535,16 +9544,16 @@
         <v>159</v>
       </c>
       <c r="I37" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="J37" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="K37" s="0" t="s">
         <v>24</v>
       </c>
       <c r="O37" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="39" s="28">
@@ -10155,7 +10164,7 @@
         <v>188</v>
       </c>
       <c r="K40" s="28" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="O40" s="28" t="s">
         <v>34</v>
@@ -10735,7 +10744,7 @@
         <v>190</v>
       </c>
       <c r="K41" s="28" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="O41" s="28" t="s">
         <v>116</v>
@@ -11315,7 +11324,7 @@
         <v>23</v>
       </c>
       <c r="K42" s="28" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="L42" s="29"/>
       <c r="O42" s="28" t="s">
@@ -11941,7 +11950,7 @@
         <v>193</v>
       </c>
       <c r="O43" s="28" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="Q43" s="25"/>
       <c r="R43" s="25"/>
@@ -14258,7 +14267,7 @@
         <v>202</v>
       </c>
       <c r="K47" s="28" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="O47" s="28" t="s">
         <v>34</v>
@@ -14835,13 +14844,13 @@
         <v>184</v>
       </c>
       <c r="J48" s="28" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K48" s="28" t="s">
         <v>24</v>
       </c>
       <c r="O48" s="28" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="Q48" s="25"/>
       <c r="R48" s="25"/>
@@ -15418,7 +15427,7 @@
         <v>122</v>
       </c>
       <c r="K49" s="28" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="O49" s="28" t="s">
         <v>34</v>
@@ -15998,7 +16007,7 @@
         <v>206</v>
       </c>
       <c r="K50" s="28" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="O50" s="28" t="s">
         <v>34</v>
@@ -18901,7 +18910,7 @@
         <v>118</v>
       </c>
       <c r="K55" s="28" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="O55" s="28" t="s">
         <v>34</v>
@@ -19481,7 +19490,7 @@
         <v>186</v>
       </c>
       <c r="K56" s="28" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="O56" s="28" t="s">
         <v>34</v>
@@ -20061,7 +20070,7 @@
         <v>190</v>
       </c>
       <c r="K57" s="28" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="O57" s="28" t="s">
         <v>34</v>
@@ -20641,7 +20650,7 @@
         <v>23</v>
       </c>
       <c r="K58" s="28" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="L58" s="29"/>
       <c r="O58" s="28" t="s">
@@ -21264,10 +21273,10 @@
         <v>192</v>
       </c>
       <c r="K59" s="28" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="O59" s="28" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="Q59" s="25"/>
       <c r="R59" s="25"/>
@@ -21844,7 +21853,7 @@
         <v>195</v>
       </c>
       <c r="K60" s="28" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="O60" s="28" t="s">
         <v>34</v>
@@ -23581,13 +23590,13 @@
         <v>216</v>
       </c>
       <c r="J63" s="28" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K63" s="28" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="O63" s="28" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="Q63" s="25"/>
       <c r="R63" s="25"/>
@@ -24164,7 +24173,7 @@
         <v>122</v>
       </c>
       <c r="K64" s="28" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="O64" s="28" t="s">
         <v>34</v>
@@ -24744,7 +24753,7 @@
         <v>212</v>
       </c>
       <c r="K65" s="28" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="O65" s="28" t="s">
         <v>34</v>
@@ -25907,7 +25916,7 @@
         <v>118</v>
       </c>
       <c r="K67" s="28" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="O67" s="28" t="s">
         <v>34</v>

</xml_diff>